<commit_message>
Address main issues from https://github.com/IPBES-Data/IPBES_TCA_Ch5_subsidies_reform/issues/3
</commit_message>
<xml_diff>
--- a/data/ch_5_subsidies_reform/random_50_subsidies.xlsx
+++ b/data/ch_5_subsidies_reform/random_50_subsidies.xlsx
@@ -387,1310 +387,1241 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2888982123</t>
+          <t>https://openalex.org/W4210477922</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1007/978-3-319-98681-4_9</t>
+          <t>https://doi.org/10.5958/2278-4853.2021.01180.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Smith et al. (2018)</t>
+          <t>Batar (2021)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ensuring Co-benefits for Biodiversity, Climate Change and Sustainable Development</t>
+          <t>A socio-legal study of police atrocities</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Significant investments are required by Parties to the three Rio Conventions—Convention on Biological Diversity (CBD), the United Nations Framework Convention on Climate Change (UNFCCC) and the United Nations Convention to Combat Desertification (UNCCD), as well as the United Nations 2030 Agenda for Sustainable Development (2030 Agenda), to meet the ambitious goals that countries have agreed to. When the development of national and subnational frameworks to meet global commitments are conducted in isolation, the opportunity is lost to: (1) leverage co-benefits from the same investment; (2) use resources more efficiently; and (3) ensure that one action does not negatively affect another policy priority. For example, investments in greenhouse gas reduction have the potential either to positively impact biodiversity and sustainable development, or to result in unintended negative consequences; chances of positive synergies are greatly increased by cooperation and joint policy, planning and implementation. The challenge now is to learn lessons from the vast and diverse number of approaches being tried around the world and to enhance co-benefits. This paper describes the major inter-linkages between global commitments for conservation and development. It demonstrates the importance of enhancing synergies among global agreements and avoiding unintended and negative consequences, particularly on biodiversity, by providing examples of best practices and describing some of the pitfalls that occur when implementation of one agreement does not explicitly seek to enhance co-benefits with other agreements. In conclusion, the paper presents the case for the central role of nature-based solutions in simultaneously attaining global commitments for biodiversity, climate change and sustainable development.</t>
+          <t>This article focuses on the intentional approach on compensating and rehabilitating victims of severe abuse. This work investigation is divided into five parts. From the very beginning of the issue, ’Police Outrages,’ the investigation breaks down the previous correct previously given to the victims of police brutality, at all levels, and moves toward the remuneration and recovery strategy which could be available for the survivors of police atrocities, while contacting and discussing the Human Rights Groups and other gatherings’ investments. The ’Police Atrocities’ include random Lathi charges on crowds, counterfeit captures, counterfeit experiences, custodial brutality, custodial, death, custodial assault and attack on women, various types of provocations while dealing with the standard guilty party, arrestees, and occasionally inconsiderate conduct and cruel treatment of blameless residents as well. Despite this, police officers engage in illegal activities and take a number of dubious and unethical actions, particularly while acting in the role of maintaining lawfulness. These and other types of human-rights violations occur on a daily basis as a result of police authority, prompting a man of ordinary reason to consider drastic reforms in the police structure. The investigation would include few suggestions, as it was seen, while the investigation was conducted for insurance against police violence, pay, and recovery methods.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2151484172</t>
+          <t>https://openalex.org/W2387150604</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ecco et al. (2012)</t>
+          <t>Lv &amp; Iron (2008)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Spatial variability of soil resistance to penetration in the area cultivated with sugar cane in the 2008/2009 season</t>
+          <t>Industry Waste Water Reformation of Sinter Plant</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The physical indicators of soil quality evaluation parameters are the possible environmental changes in soil-plant system. The sugar cane is a crop of great importance for the state of Mato Grosso do Sul, and studies that assess the possible changes of soil to assist in the sustainability of the production system and environment are of utmost importance. In this sense, the experiment aimed to apply geostatistical techniques to study the spatial variability of the soil resistance to penetration (RMP), the management system of mechanized harvesting of cane sugar, in layers from 0 to 0.20 me 0.20 to 0.40 m. The experiment was conducted at the Plant ETH Bioenergy, Rio Bright-MS, over an Oxisol. The experimental design in the plot consisted of 144 samples point over an experimental grid. The determination of the PMR was performed using an impact penetrometer. The spatial variability in soil and the RMP of each layer of the sugarcane field was determined using geostatistical techniques. The semivariograms were elaborated and applied to the kriging interpolation process. It was found that the dependence of 176 m and 30 m, respectively for the layers of 0-0.20 and 0.20-0.40 m RMP in the upper layer showed more homogeneous areas than the lower layer and can thus be adopted a different management systems between these layers of soil.</t>
+          <t>Because of super-alkalic waste discharge of sinter plant,then pollute the TaiZi river quality, the reduction of water consumption was adopted by sinter plant, and reformed the waste-water treatment tank. After purification, as adding water into the mixing at the middle of it instead of new water.Industry waste closed-circuit and waste zero discharge were obtained .</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2129272042</t>
+          <t>https://openalex.org/W4239824631</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/s0140-6701(04)91357-4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Damanski (1998)</t>
+          <t>NA (2004)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Monitoring land quality : assuring more sustainable agricultural production systems</t>
+          <t>04/00155 Heat pipe-based cooling system in reforming and steam reforming of hydrocarbons in manufacture of fuel cell-grade hydrogen</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Identification of Land Quality Indicators (LQIs) is a key requirement of sustainable land management. They are required to assess, monitor, and evaluate changes in the quality of land resources and environmental impacts. The Land Quality Indicator (LQI) program monitors the environment and the sector performance of managed ecosystems. The program is being developed on a national and regional scale, but it is also part of a larger global effort to improve natural resource management. The LQI program recommends addressing issues of land management by agroecological zones. This approach favors incorporating farmer knowledge into the overall process of improving agricultural and environmental land management. The LQI approach focuses on preventive maintenance rather than rehabilitation.</t>
+          <t>Apoptosis resistance in melanoma is a primary cause of treatment failure. Apoptotic pathways in melanocytes, from which melanoma arises, are poorly characterized. Human melanocytes were susceptible to apoptosis following exposure to UV radiation (UVB, 24–48 hours), 4-tert-butylphenol (4-TBP, 1–4 hours), and cisplatin (24–48 hours). These responses were associated with Bid cleavage, caspase activation (caspases 3, 8, and 9), mitochondrial depolarization and release of cytochrome c, Smac/DIABLO, and apoptosis-inducing factor (AIF), but not endonuclease G. The apoptotic responses and AIF release were caspase-independent, as they were not blocked by zVal-Ala-Asp(OMe)-fluoromethyl ketone (zVAD-fmk). While RNA interference-mediated knockdown of AIF protected melanocytes against apoptosis induced by serum withdrawal, apoptotic responses to UVB, cisplatin, and 4-TBP were not compromised by AIF knockdown, even in the presence of zVAD-fmk. Finally, adenoviral-mediated expression of Survivin, an inhibitor of apoptosis expressed in melanoma but not melanocytes, protected melanocytes against UVB-induced apoptosis. Survivin expression in melanocytes partially blocked caspase activation and release of mitochondrial release of AIF, cytochrome c, and Smac induced by UVB. These data indicate that multiple stimuli can activate both caspase-dependent and caspase-independent apoptotic pathways in melanocytes, and that endogenous expression of Survivin in melanoma may contribute to apoptosis resistance by multiple mechanisms.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1256015070</t>
+          <t>https://openalex.org/W2936109454</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.24919/2308-4634.2019.163121</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hu et al. (2007)</t>
+          <t>Kravchenko (2019)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emergy evaluation of the artificial forest ecosystems in the watershed of Miyun Reservoir：a case study for ecosystems valuation and environmental management</t>
+          <t>ПРOФЕСIO-ПСИХOГРAМA (IНФOРМAЦIЙНO-КOМУНIКAЦIЙНИЙ AСПЕКТ) ПРOФЕСIЙНOЇ ПIДГOТOВКИ МAЙБУТНIХ OФIЦЕРIВ ЗБРOЙНИХ СИЛ УКРAЇНИ</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>The structure of a professional specialist is considered in the article. The structure of the professional specialist is a system-forming factor in building a process for the training of future officers of the Armed Forces of Ukraine. Psychophysiological aspect of any professional activity of a person (including an officer of the Armed Forces) is disclosed through the description of requirements. These requirements are put forward to the military to provide military capability and combat readiness of the military subdivision.The professional qualification (aspect of information and communication competence) of the future officer of the Armed Forces of Ukraine is aimed at creating an information, motivational basis for the future officer’s officer in the conditions of the military conflict in the east of the state. The goal is also to reform and modernize the Armed Forces of Ukraine.The main functions performed by a professional officer are deeply analyzed: informational, diagnostic, predictive, forming.It is determined that the psychogram is the basis for constructing a psychological portrait of the officer’s face. Principles of constructing a psychological portrait of an officer should be used both in the process of professional removal of future military, and in the official characteristics of the officerf.As a result of expert research, the psychic characteristics of an officer were determined. These characteristics are formed during the learning process. The officer’s psychogram is created (psychological portrait). Also, the role of various professionally important qualities of the future activity of the soldier is revealed. The characteristic (psychological portrait of a person) can be a reliable basis for an adequate assessment of an officer and prediction of his professional efficiency and possible projected career growth.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4206408028</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.4324/9780429324680-2</t>
+          <t>https://openalex.org/W2763993878</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pacudan (2021)</t>
+          <t>Alvesson et al. (2017)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Whole-of-nation approach to climate change governance in Brunei Darussalam</t>
+          <t>Return to Meaning: A Social Science with Something to Say</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>This chapter provides presentation of the government’s rationale for climate change intervention, discussion of the national challenges in the transition to a low carbon and climate-resilient economy, presentation of the whole-of-nation approach in policy formulation, presentation of the policy strategies, and discussion of potential challenges and the governance implications in policy implementation. Brunei Darussalam is situated on the northwest coast of the island of Borneo, with flat coastal plains and an equatorial climate. The country faces various financial and technical challenges in achieving a balanced mix of measures that satisfies multiple developmental concerns. Brunei pursues an energy pricing policy that sets energy prices, in the case of petroleum products, below the international market reference prices or, in the case of electricity services, below the long-run marginal cost. In the process of preparing the Brunei Climate Change Policy, the Brunei Climate Change Secretariat updated the greenhouse gas inventory.</t>
+          <t>This book argues that we are currently witnessing not merely a decline in the quality of social science research, but the proliferation of meaningless research, of no value to society, and modest value to its authors - apart from securing employment and promotion. The explosion of published outputs, at least in social science, creates a noisy, cluttered environment which makes meaningful research difficult, as different voices compete to capture the limelight even briefly. Older, more significant contributions are easily neglected, as the premium is to write and publish, not read and learn. The result is a widespread cynicism among academics on the value of academic research, sometimes including their own. Publishing comes to be seen as a game of hits and misses, devoid of intrinsic meaning and value, and of no wider social uses whatsoever. Academics do research in order to get published, not to say something socially meaningful. This is what we view as the rise of nonsense in academic research, which represents a serious social problem. It undermines the very point of social science.This problem is far from 'academic'. It affects many areas of social and political life entailing extensive waste of resources and inflated student fees as well as costs to tax-payers. Part two of the book offers a range of proposals aimed at restoring meaning at the heart of social research and drawing social science back address the major problems and issues that face our societies. (Less)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4390097584</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1109/powerafrica57932.2023.10363321</t>
+          <t>https://openalex.org/W2260697321</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sam et al. (2023)</t>
+          <t>Auray &amp; Eyquem (2014)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Integration of Green Mobility in Niche Markets in Morocco</t>
+          <t>War, Taxes and Trade</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>The transport sector plays a major role in the global energy consumption and is responsible for a significant share of greenhouse gas emissions worldwide. Thus, decarbonization of this sector has become imperative. Electric and hydrogen vehicles are effective green mobility solutions to achieve this goal. In this sense, the present study examines the implementation of green mobility solutions in Morocco, focusing on the use of buses in different niche markets. To do so, the ADVISOR software was used to model the work and compare the Key Performance Indicators (KPI) that are crucial for selecting the best solution. The objective is to evaluate the performance of these vehicles on two driving cycles, representative of urban and extra urban driving. According to the results, it was found that the electric and hydrogen vehicles could be more competitive than the diesel vehicles in addition to zero CO &lt;inf xmlns:mml="http://www.w3.org/1998/Math/MathML" xmlns:xlink="http://www.w3.org/1999/xlink"&gt;2&lt;/inf&gt; emissions.</t>
+          <t>those with low levels. Consequently, the latter should play better than predicted and(This abstract was borrowed from another version of this item.)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4210452534</t>
+          <t>https://openalex.org/W3136902462</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.apenergy.2021.118447</t>
+          <t>https://doi.org/10.1093/bjsw/bcab047</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Casalicchio et al. (2022)</t>
+          <t>Choate (2021)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>From investment optimization to fair benefit distribution in renewable energy community modelling</t>
+          <t>The Politics of Children’s Services Reform: Re-Examining Two Decades of Policy Change, Carl Purcell</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Energy communities are becoming a key topic in the decarbonization process as they can simultaneously guarantee economic, environmental, and social benefits. In this paper, an integrated method for the implementation of a linear bottom-up optimization model has been developed in order to address these aspects of an energy community: (i) definition of the dispatch and the best technology mix; (ii) assessment of the role of the Demand Side Management; (iii) definition of an original and fair method to allocate the benefit among the participants and of a Fairness Index to compare different business models. The developed method has been applied to an illustrative case study through the implementation of the Italian regulatory framework definitions and costs. The outcomes highlight how Demand Side Management and the energy community composition of the energy community impact on the overall investment: a case study, with heterogeneous composition and characterized by a 20% of flexible load, presents a reduction of 13% in photovoltaic and 93% in storage system capacity with respect to the case without Demand Side Management. The renewable source consumption with a more homogeneous case study decreases by around 20%–33% and bill savings by around 30%. These results impact also on each participant contribution, which underpins the introduced fair distribution method. Leading thus to a different and more proper distribution of the benefit, in order to guarantee everyone the fairest economic return. Moreover, a Fairness Index has been introduced to assess the consistency of other Business Models with respect to the fair distribution.</t>
+          <t>There is no denying that politics, politicians and political agendas have had a profound impact on personal services for several decades (Jones, 2020). Purcell takes us through an insightful journey of the particular role that specific governments can have, but, perhaps most importantly, how the agendas of politicians can affect the course, funding and priorities of children’s services. Purcell presents a thorough and coherent story about how agendas are managed, implemented and funded, while helping the reader to understand the power of the central government to set targets that local administrations must grapple with. Purcell has laid the chapters out into two vibrant sections. The first looks at the reforms under the Labour Governments of 1997–2010 while the second looks at the coalition and Conservative governments of 2010–2019. The strength of these period reviews is the draw upon primary sources and interviews of key players. The reader thus...</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2225253261</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.2139/ssrn.2509888</t>
+          <t>https://openalex.org/W2993769636</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Widenhorn (2013)</t>
+          <t>Oh (2011)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Braving the Storm: How are Global Biofuel Policies Sustained Despite Being Contested? An Analysis of the Biofuel Discourses of the EU, Brazil and Mozambique</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Considered as a remedy to multiple problems that our world is facing, biofuels are nowadays promoted on a global scale. Despite this globalised approach, however, biofuels are heavily contested. Not only the social implications of biofuels are disputed and uncertain, particularly in countries of the global South, but also their environmental and economic rationales. Given these huge controversies, policies promoting biofuels would seem difficult to maintain. Yet, support for them has been surprisingly well established on the political agendas. With the aim of understanding this puzzle, this study asks how the dominant approach to biofuels has been sustained on a global level. In order to answer this question, the meanings and assumptions in biofuel discourses are explored through the lens of Maarten Hajer’s “argumentative” discourse analysis. Based on the existence of a “partnership for sustainable bioenergy” between the EU, Brazil and Mozambique, the study takes these three locations as case studies. The analysis reveals that various discursive strategies, including a particular problem construction and the use of two main story-lines, have played an important role in ensuring the permanence of the global approach to biofuels. Moreover, while the discourse of critics against biofuels demonstrates that there is room for contestation, the analysis finds that the opponents’ discourse largely fails to target the most salient justification for biofuels. A more effective strategy for critics would therefore be to also question the problem constructions underpinning this main justification in the global discourse.</t>
+          <t>The Study of Gongbeop of King Sejong the Great and Thoughts on Taxation －From the Perspective of Tax Law－</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2251239228</t>
+          <t>https://openalex.org/W3106244966</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.enpol.2009.11.038</t>
+          <t>https://doi.org/10.1177/0031512520972879</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Villemeur &amp; Pineau (2010)</t>
+          <t>Costa et al. (2020)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Environmentally damaging electricity trade</t>
+          <t>Effects of Cognitive Over Postural Demands on Upright Standing Among Young Adults</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Electricity trade across regions is often considered welfare enhancing. We show in this paper that this should be reconsidered if environmental externalities are taken into account. We consider two cases where trade is beneficial, before accounting for environmental damages: first, when two regions with the same technology display some demand heterogeneity; second when one region endowed with hydropower arbitrages with its “thermal” neighbor. Our results show that under reasonable demand and supply elasticities, trade comes with an additional environmental cost. This calls for integrating environmental externalities into market reforms when redesigning the electricity sector. Two North American applications illustrate our results: trade between Pennsylvania and New York, and trade between hydro-rich Quebec and New York.</t>
+          <t>A growing body of research has shown that static stance control (e.g., body sway) is influenced by cognitive demands (CD), an effect that may be related to competition for limited central resources. Measures of stance control have also been impacted by postural demands (PD) (e.g., stable vs. unstable stances). However, less is known of any possible interactions between PD and CD on static stance control in populations with intact balance control and ample cognitive resources, like young healthy adults. In this study, among the same participants, we factorially compared the impact of PD with and without CD on static stance control. Thirty-four healthy young adults wore inertial measurement units (IMU) while completing static stance tasks for 30 seconds in three different PD positions: feet apart, feet together, and tandem feet. After completing these tasks alone, participants performed these tasks with CD by concurrently completing verbal serial seven subtractions from a randomly selected three-digit number. For two dependent measures, path length and jerk, there were main effects of CD and PD but no interaction effect between these factors. For all other stance control parameters, there was only a PD main effect. Thus, adding a cognitive demand to postural demands, while standing upright, may have an independent impact on stance control, but CD does not seem to interact with PD. These results suggest that young healthy adults may be less sensitive to simple PD and CD due to their greater inherent balance control and available cognitive resources. Future work might explore more complex PD and CD combinations to determine the boundaries under which young adults’ resources are taxed.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2169898895</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.envsci.2012.02.001</t>
+          <t>https://openalex.org/W2350598797</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pirard (2012)</t>
+          <t>Wang (2015)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Market-based instruments for biodiversity and ecosystem services: A lexicon</t>
+          <t>Research on the Development of Non-Olympic Events in China from the Perspective of Institutional Change</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Although market-based instruments (MBIs) gained prominence in discourses and practice in the field of biodiversity conservation and provision of ecosystem services, their definition and underpinning theory still are unsettled matters. A review of MBIs – including payments for ecosystem services, taxes and subsidies, mitigation or species banking, certification, etc. – clearly shows that this label encompasses an extremely diverse array of instruments. Their only shared characteristic might be the attribution of a price to nature, yet in different ways and not necessarily in conjunction with economic valuations of the benefits/impacts associated with biodiversity and ecosystem services. Their links with markets are often loose, at least contrasted if not questionable in many cases. This pleads for a better lexicon of such a large collection of policy instruments in order to better inform policy making. This lexicon is based on the links between MBIs, economic theory, and markets. It includes six generic categories: regulatory price signals, Coasean-type agreements, reverse auctions, tradable permits, direct markets, and voluntary price signals. As a matter of illustration, “Payments for Ecosystem Services” refer to various instruments in the literature and in practice. Depending on the context they could fit in all of our categories but one, so that we wonder if the term itself is not emptied of any useful meaning at least from an operational perspective. Last, the diversity of MBIs with regard to their functioning and links with markets seems to disqualify any general statement, be it in favour or against their development. In particular, MBIs as a whole cannot be said to be cost-efficient, risky, inequitable, or capable of revealing information to reach a social optimum and better environmental management.</t>
+          <t>Based on the theory of institutional change,this paper makes an analysis on the sports rights game between Olympic events and non-Olympic events.It points out that Olympic events are the products of supply-oriented institutional change,while non-Olympic events are the choice of demand-oriented institutional change.At the same time,the development of non-Olympic events is a major institutional change process that bears the feature of path dependence,which may consolidate and strengthen the achievements and influences that theWhole Nation Systemhas obtained.The new system reform and innovation may encounter much resistance,which makes it a long way to go for the development of non-Olympic events.To solve the problem of path dependence is the key to develop non-Olympic events,which can accelerate the process of institutional reform and power release as well as clear away the obstacles of sports system reform.The leading role of the General Administration of Sport in the reform should be placed on supporting both the advantaged and disadvantaged events.In addition,the development of non-Olympic events should rely on the special role of ideology in the reform,which directly decides the direction of the sports development in China.Finally,the path choice of non-Olympic events reorganization is put forward in the study.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2800234244</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.3390/su10041254</t>
+          <t>https://openalex.org/W38870991</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Islam et al. (2018)</t>
+          <t>Damiani et al. (2015)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Social Considerations of Large River Sanctuaries: A Case Study from the Hilsa Shad Fishery in Bangladesh</t>
+          <t>[Features and developments of Primary Care in a Public Health perspective].</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>The establishment of a sanctuary is often suggested as an effective strategy for ecological restoration, though social aspects of such attempts are often overlooked. This study analyzed the socioeconomic status of 248 fishing households who are dependent on hilsa shad (Tenualosa ilisha) sanctuaries in southern Bangladesh. Also, the fishers&amp;rsquo; perceptions were investigated to assess the status of ecological restoration, level of participation in the hilsa sanctuary management, their livelihoods constraints, and coping strategies during crises. Based on the fishers&amp;rsquo; perceptions and fishery catch data of the government, it appears that the establishment of the hilsa sanctuary in the Bangladesh waters helped to restore the hilsa fishery and also enhanced the fishers&amp;rsquo; income. However, a large section of hilsa fishers were found to be poor in terms of socioeconomic capital such as monthly income, housing conditions, and assets ownership. Particularly, these households suffer seasonal food insecurity during the banned period of fishing in the sanctuaries. The government&amp;rsquo;s compensation scheme is a good example of payment of ecosystem services in an open water fishery; however, this scheme does not include all the affected fishers. Food and income insecurity during ban period often force fishers to use illegal fishing as a livelihood strategy that undermines the success of sanctuaries as an ecological restoration strategy. The findings reflected that sanctuaries and other similar management strategies have social impacts on stakeholders and human societies, and these social impacts can have surprising feedbacks that influence management success. Thus, the success of ecological restoration relies on understanding the human dimensions of the system and that ecological and social restoration must go together. To address this goal, we call for developing fisheries policy that will facilitate engagement of resource users and other local stakeholders in sanctuary comanagement, which will ultimately strengthen fishers&amp;rsquo; livelihoods and sustain the benefit from ecological restoration.</t>
+          <t>In recent years, substantial changes of the population structure have occurred, both at the national and international levels, due to several factors, including demographic changes and technological progress. At the same time, an epidemiological transition is occurring, characterized by a shift from diseases with an acute onset and a rapid resolution, to chronic-degenerative conditions which require more long-term care solutions. This shift seems to contribute to an increased life expectancy of the population, and a larger proportion of elderly individuals having complex health needs. The above described changes of the population structure, in combination with the current economic and financial crisis, require a redefinition of health system priorities at different levels, and the identification of specific intervention approaches. Today Primary Care is generally considered to have a key role in the progress of health systems and governments and international agencies, including the World Bank and the World Health Organisation have already increased investments and introduced reforms of Primary Care. However, there still remains much to be done, particularly with regards to the definition of specific aspects related to Primary Care. In this article the characteristics and developments of two main concepts, Primary Care (PC), which describes the delivery of Primary Care services, and Primary Health Care (PHC), which is more broadly defined by a level of governance or stewardship, are described. The distinction between PC and PHC implies the need for a characterization of system governance or stewardship, and of governance for care delivery. The first entails decision-making mechanisms for protecting the health both of individuals and of communities, by setting health, appropriateness and economic sustainability goals. These decisionmaking mechanisms further take into account the consequent responsibilities and risks compared to the achieved results toward citizens. The second relates to decision-making mechanisms for the delivery of services. Some examples are given of the application of system governance for primary healthcare at the national level and of characteristics of aggregations of professionals and/or structures for PC delivery. Finally, ideas and proposals for the development of an integrated approach for the delivery of Primary Care and prevention services, in a Public Health perspective are presented.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4390717553</t>
+          <t>https://openalex.org/W2955930990</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.cities.2023.104751</t>
+          <t>https://doi.org/10.5089/9781451851120.001</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Alves et al. (2024)</t>
+          <t>Gordon (1997)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Planning the multifunctionality of nature-based solutions in urban spaces</t>
+          <t>Do Tax Rates Encourage Entrepreneurial Activity?</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Urban infrastructure is under substantial stress due to climate change and urbanisation. More frequent flooding events and heat waves in cities threaten citizens' health and wellbeing. Current infrastructure is mostly based on grey solutions, focusing on only one function. Nature-based solutions (NBS), which are supported by nature and mimic natural processes, are multifunctional and can provide several benefits at the same time. However, this multifunctionality is deficiently considered during planning of urban infrastructure transitions. This work presents a method to help urban NBS planning processes considering multiple climate adaptation objectives. It is a 3-steps GIS-based multi-criteria method, in which the first step is a “priority areas identification”, the second step is a “site-specific NBS allocation”, and the third step is a “multifunctional performance evaluation”. The method was applied to a case study to demonstrate its operation and validate the outcome with stakeholders. This work helps to improve the planning of multifunctional NBS in cities considering local needs, spatial opportunities, and site-specific limitations. Furthermore, it allows to assess the trade-offs among multiple NBS benefits when more than one objective is pursued.</t>
+          <t>When the top personal tax rates are above the corporate rate, high-income individuals have an incentive to reclassify their earnings as corporate rather than personal income for tax purposes. U.S. tax law at least imposes strict limits on the extent to which employees in publicly traded corporations can engage in such income shifting. However, entrepreneurs setting up new firms can easily reclassify their income for tax purposes. This tax incentive therefore favors entrepreneurial activity. The paper discusses how best to subsidize entrepreneurial activity while avoiding other economic distortions.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3135306210</t>
+          <t>https://openalex.org/W3092509142</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://doi.org/10.4000/rei.11641</t>
+          <t>https://doi.org/10.7176/jlpg/101-18</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Littlejohn &amp; Proost (2022)</t>
+          <t>Supriyanto &amp; Krismantoro (2020)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>How to be a good forerunner in carbon neutral trucking</t>
+          <t>Juridical Review of The Complete Systematic Land Registration in Indonesia</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>EU countries want to decarbonize their road freight transport quickly. Long-haul electric trucks are a promising technology. There are several competing designs but at present the trade-off is between e-trucks with very large batteries and e-trucks with a smaller battery but combined with motorways electrified via catenary lines. In the latter case a combination of public investment (catenary lines on major motorways) and private investment (electric trucks) is required. As long-haul truck transport is partly international this raises problems of coordination among countries. We study the possible pricing and investment strategy of one forerunner country that faces lagging neighbors. The forerunner can make the use of electric trucks mandatory on its own territory by using very high road charges for diesel trucks. If it has opted for a catenary system, it faces still the choice of how it will price the use of its electric motorways. International diesel trucks, when crossing the border of a forerunner country, must choose between paying high charges and transferring the load into an e-truck. We study the outcome of this international coordination game exploring the non-cooperative outcome varying the relative size of the forerunner in international truck traffic. The same investment coordination is present when one counts on a combination of more dense and cheaper batteries with fast chargers. It is the country with the smallest appetite for decarbonized trucking that will dictate the development in international electric trucking.JEL classification: Q54, Q55, Q58, R42, R48.</t>
+          <t>The Complete Systematic Land Registration (PTSL) activity is a Government program to achieve legal certainty and the existence of a single map in Indonesia. Therefore, the target of PTSL is land that does not have a certificate in one village. Prior to the PTSL activity, there was an activity called the National Agrarian Operation Project (PRONA). These activities were not successful, so there was a new land registration system called PTSL. The methods used in this research are normative and empirical juridical methods. The results of a study on the implementation of Complete Systematic Land Registration (PTSL) in Indonesia show that it has provided legal certainty to land owners. However, in implementing PTSL in Indonesia, there are still obstacles in the implementation of PTSL. These obstacles include the lack of adequate human resources to support the implementation of PTSL, the lack of facilities and infrastructure for implementing PTSL in the regions, the lack of full support from the community for PTSL activities, and the large tax costs on land owned by the community. Keywords: juridical review, complete systematic registration, legal certainty DOI: 10.7176/JLPG/101-18 Publication date: September 30 th 2020</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4366966834</t>
+          <t>https://openalex.org/W4252975685</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1007/978-981-19-7506-6_17</t>
+          <t>https://doi.org/10.1146/annurev.soc.18.1.519</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sivarathnakumar et al. (2023)</t>
+          <t>Lubeck (1992)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Ecological and Economic Impacts on Biofuel Production</t>
+          <t>The Crisis of African Development: Conflicting Interpretations and Resolutions</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>This chapter addresses the issues and impact of biofuel production in environment and economic aspects of bioenergy. In case of biofuel production, biogas, biodiesel, bioethanol are the most predominant products produced which utilises food crops/grains, lignocellulosic biomass as raw materials. This leads to significant impact on environmental aspects like agricultural land usage, food to fuel competition, food security, greenhouse gas emission, trade of biofuel water and biodiversity. It also has a huge impact on the economic aspects like energy security, employment opportunities and also on human health. The feasibility of biofuel production can be made sustainable only if the environmental and economic aspects are addressed properly.</t>
+          <t>The depth and duration of economic decline, coupled with ecological degradation, political paralysis, and institutional decay, has created an unprecedented crisis in sub-saharan Africa. Explanations for the multiple crises of African development focus on debates regarding the necessity of following market-oriented economic policies, the capacity of African states to manage either development or reform and the way in which African institutions reproduce societies that are resistant either to state-centered development or to market forces. After allowing for events that are beyond the control of policy, the three schools—neoliberal, structural-nationalist, and institutional—are used to evaluate the literature on peasant agriculture, industry, and state policy. The experience of Nigeria indicates that commercial agriculture is increasing, that structural reforms can have some positive benefits and that its hydrocarbon sector can form a basis for regional industrialization. Finally, the rise of popular democratic movement suggests how the crisis has unleashed elements of a formerly passive civil society which promise to reform authoritarianism and discipline rentier states.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3211390895</t>
+          <t>https://openalex.org/W4367029550</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1007/978-3-662-63760-9_29</t>
+          <t>https://doi.org/10.1515/9781685859589-007</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Agresti et al. (2021)</t>
+          <t>NA (1994)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Modeling Chain Set up for the Assessment of Policy Impacts on Air Quality and Human Health</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Private road transport segment is one of the main contributors to poor air quality, especially in densely populated cities. This study aims to simulate future mobility scenarios on the Italian peninsula and the associated impacts. A modeling chain composed by several modules is implemented to perform this analysis and the implications of a Reference and a Decarbonization scenarios are discussed. The first module is composed by an energetic model which outlines the car fleet evolution in terms of composition, vehicles kilometres travelled (VKT) and energy consumptions in 2030. A novel methodology is then applied to the energy model output to infer the private road transport emission variation respect to the base case year (2010). Then the estimation of the scenario’s atmospheric concentration of NO2, PM2.5 and O3, over a whole year, is obtained by means of a chemical transport model. Finally, some estimates of the health impact of two scenarios are provided, based on the variation of PM2.5 and O3 simulated concentration, respect to the base case year. Both scenarios expect an increase of the total demand for private transport in 2030 (18% for the Reference one), but at the same time a reduction of ICE cars in favour of hybrid and electric vehicles, with respect to the base case year. This trend leads to a general improvement of air quality, especially for the Decarbonization scenario for which the reduction of NO2 concentration reaches 25% in some areas.</t>
+          <t>4 THE IMPACT OF OTTOMAN REFORMS AND WESTERN ECONOMIC EXPANSION, 1875-1908</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2089128369</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1289/ehp.120-a346</t>
+          <t>https://openalex.org/W2550765579</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Schmidt (2012)</t>
+          <t>Galjart (1971)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>The Endocrine Society Issues Statement of Principles</t>
+          <t>Politieke mobilisatie van boeren in Latijns Amerika</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Vol. 120, No. 9 News | ForumOpen AccessThe Endocrine Society Issues Statement of Principles Charles W. Schmidt Charles W. Schmidt Search for more papers by this author Published:1 September 2012https://doi.org/10.1289/ehp.120-a346View Article in:中文版AboutSectionsPDF ToolsDownload CitationsTrack Citations ShareShare onFacebookTwitterLinked InReddit A new position statement from The Endocrine Society provides a strong argument for scientists in industry, government, and academia to work together, across disciplines, to improve testing of chemicals as potential endocrine disruptors. Published ahead of print in Endocrinology on 25 June 2012,1 the statement focuses on the Environmental Protection Agency’s (EPA) Endocrine Disruptor Screening Program (EDSP) to illustrate how fundamental endocrinology principles might be incorporated into more rigorous screens for endocrine activity. But according to lead author R. Thomas Zoeller, a biology professor at the University of Massachusetts, Amherst, the need for broader consideration of endocrinology extends to screening programs beyond the EDSP.The EDSP flags potential endocrine disruptors with a two-tiered system. Tier 1 assays, which were validated by the Federal Insecticide, Fungicide, and Rodenticide Act Science Advisory Panel in 2008,2 provide information for use in identifying chemicals that could potentially interact with the endocrine system. Tier 2 assays, which are currently undergoing validation, evaluate dose responses between those interactions and chemical exposure. The Endocrine Society statement focuses on Tier 1, which employs a variety of in vitro and in vivo assays with a long history in toxicology.Given that they mimic hormones, endocrine disruptors don’t behave like other toxicants, Zoeller explains. Chemical effects generally increase with greater exposure, but hormones rarely display dose linearity. That’s because if a hormone saturates its receptor, more of the same hormone will have no greater effect on response. And in some cases, high doses downregulate responses triggered by lesser exposures—in other words, different effects can appear and disappear at different doses. These “nonmonotonic” dose–response curves—commonly accepted in endocrinology—challenge a fundamental premise of toxicology: that chemical effects become more pronounced with increasing dose.The Endocrine Society’s view is that exposure levels employed in the EDSP’s Tier 1 assays—which start with the maximum tolerated doses identified in previous toxicology testing, then work their way down—are so high as to potentially miss low-dose, nonmonotonic effects. But Lorenz Rhomberg, principal at Gradient Corporation, an environmental risk assessment firm in Cambridge, Massachusetts, counters that Tier 1 tests were designed solely to test for endocrine system interactions, so the dose doesn’t matter. “Questions about dose response are dealt with in Tier 2,” he says. In response to e-mailed questions regarding the EDSP, an EPA spokesman3 writes that the Agency’s Office of Research and Development is “developing a review of the state of the science on low-dose, nonmonotonic dose–response curves and its potential impact on . . . risk assessment.”The definition of the term “endocrine disruption” is an important factor in determining the evidence needed to identify a chemical as an endocrine disruptor. The World Health Organization (WHO) and the European Union define endocrine disruptors specifically as causing adverse effects in organisms, whereas the EPA and the WHO cite specific mechanisms by which endocrine disruption occurs. The Endocrine Society, on the other hand, proposes a streamlined version of the EPA’s 1996 definition of an endocrine disruptor to include “exogenous chemicals or chemical mixtures that interfere with any aspect of hormone action,” irrespective of adverse effects or specific mechanisms.1Given that they mimic hormones, endocrine disruptors don’t behave like other toxicants. Hormones rarely display dose linearity, and in some cases, high doses downregulate responses triggered by lesser exposures—in other words, different effects can appear and disappear at different doses.Image courtesy of U.S. EPAThe statement explains that screening only for a limited set of end points that does not reflect full understanding of endocrinology principles means bona fide endocrine disruptors could slip through undetected. For instance, by judging thyroid hormone action primarily on the presence of histopathological changes in the thyroid—which typically are a function of changes in serum levels of thyroid-stimulating hormone (TSH)—the EDSP does not recognize other important means by which the thyroid influences health. Polychlorinated biphenyls reduce levels of thyroxine but not of TSH. If these chemicals were to undergo Tier 1 testing today, they likely would not be flagged as endocrine-disrupting chemicals for study in Tier 2.1George Gray, director of the Center for Risk Science and Public Health at the George Washington University, in Washington, DC, says the proposed definition is toxicologically unorthodox. “It’s going to need a lot of scientific vetting,” he says. “This is hardly something that should be adopted by EPA without a lot of consultation with scientists both within and outside the agency.” The EPA spokesman said the agency would follow peer-review risk assessment methodology and evaluate chemicals on a case-by-case basis in its efforts to set regulatory points of departure that protect human health.A total of 67 chemicals have been selected for Tier 1 screening so far, at a cost of $500,000 each, according to the agency spokesman. The agency continues to review incoming data, but none of these chemicals—most of them pesticide active ingredients and high-production-volume chemicals used as inert ingredients in pesticide formulations—have been flagged as endocrine disruptors using current tests.References1 Zoeller RT, et al. Endocrine-disrupting chemicals and public health protection: a statement of principles from The Endocrine Society. Endocrinology; http://dx.doi.org/10.1210/en.2012-1422 [online 25 Jun 2012]. Google Scholar2 EPA. Assay Development and Validation: Tier 1 Screening Battery [website]. Washington, DC:U.S. Environmental Protection Agency (updated 11 Aug 2011). Available: http://www.epa.gov/endo/pubs/assayvalidation/tier1battery.htm [accessed 1 Aug 2012]. Google Scholar3 Current EPA practice is to attribute statements to the agency rather than to individuals. Google ScholarFiguresReferencesRelatedDetails Vol. 120, No. 9 September 2012Metrics About Article Metrics Publication History Originally published31 August 2012Published in print1 September 2012 Financial disclosuresPDF download License information EHP is an open-access journal published with support from the National Institute of Environmental Health Sciences, National Institutes of Health. All content is public domain unless otherwise noted. Note to readers with disabilities EHP strives to ensure that all journal content is accessible to all readers. However, some figures and Supplemental Material published in EHP articles may not conform to 508 standards due to the complexity of the information being presented. If you need assistance accessing journal content, please contact [email protected]. Our staff will work with you to assess and meet your accessibility needs within 3 working days.</t>
+          <t>A prerequisite for understanding the political mobilization of peasants in Latin America is an understanding of the social structure in which they live. Almost all of the arable land is in the hands of a few large landholders. Some peasants own small parcels of land; others are forced into patronage relationships with the land owners, which gives some degree of economic advantage usually paid for by loss of political power. Patronage is one reaction to the inequality of the South American peasant situation. Various forms of adaptation to inequality exist including escapism, ritualism, etc. Usually, the initiator of the mobilization process is not himself a peasant, since peasants do not have the necessary contacts and can easily be pressured by land owners. For a mobilization effort to be successful, peasants must have support in high places (persons, or organizations ie, political parties). One of the main problems facing reform efforts is that participants cannot agree as to what the specific goals and methods should be. Farm laborers are often not involved in the process at all. 1 figure. P. Tiersma.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4317653973</t>
+          <t>https://openalex.org/W2604599068</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1101/2023.01.20.524753</t>
+          <t>https://doi.org/10.21307/eb-2017-001</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Lecina‐Diaz et al. (2023)</t>
+          <t>John &amp; Robb (2017)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Incorporating fire-smartness into agricultural policies minimises suppression costs and ecosystem services damages from wildfires</t>
+          <t>Using behavioural insights for citizen compliance and cooperation</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Abstract Global climate warming is expected to increase wildfire hazard in many regions of the world. In southern Europe, land abandonment and an unbalanced investment toward fire suppression instead of prevention has gradually increased wildfire risk, which calls for a paradigm change in fire management policies. Here we combined scenario analysis, fire landscape modelling, and economic tools to identify which land-use policies would minimise the expected wildfire-related losses in a representative mountainous area of the northwestern Iberian Peninsula (the Transboundary Biosphere Reserve ‘Gerês-Xurés’, between Spain and Portugal). To do so, we applied the least-cost-plus-net-value-change approach and estimated net changes in wildfire damages based on their implications for the ecosystem services that affect financial returns to landowners in the study area (i.e. agriculture, pasture, and timber) and the wider economic benefits (i.e. recreation and climate regulation) for the 2010-2050 period. Four land-use scenarios were considered: (1) Business as Usual (BAU); (2) fire-smart, fostering more fire-resistant (less flammable) and/or fire-resilient landscapes (fire-smart); (3) High Nature Value farmlands (HNVf), wherein the abandonment of extensive agriculture is reversed; and (4) a combination of HNVf and fire-smart. We found the highest net value change (i.e. the difference between damages and avoided damages) in BAU for timber and pasture provision, and in fire-smart for recreation and climate regulation. HNVf was the best for suppression cost savings, but it generated the lowest expected present value for climate regulation. In fact, the best scenarios related to fire suppression are HNVf and HNVf combined with fire-smart, which also generate the lowest net value change plus net suppression costs in the entire study area (i.e. considering all ecosystem services damages and suppression costs). Therefore, reverting land abandonment through recultivation and promoting fire-resistant tree species is the most efficient way to reduce wildfire hazard. In this sense, payments for ecosystem services should reward farmers for their role in wildfire prevention. This study improves the understanding of the financial and societal benefits derived from reducing fire suppression spending and ecosystem services damage by undertaking fire-smart land-use strategies, which can be essential to enhance local stakeholders’ support for wildfire prevention policies. Highlights Land-use changes impact wildfire ecosystem services (ES) damages and suppression costs Promoting agriculture generates significant suppression cost savings Agriculture + fire-resistant forests is the best to reduce wildfire ES damages Land-use policies should balance trade-offs between climate and wildfire regulation Payments for ES should reward farmers for their role in wildfire prevention</t>
+          <t>Abstract In recent years, public agencies have frequently deployed behavioural insights to generate benefits for society, through encouraging citizens to comply with official requests, and more generally encouraging them to cooperate with public agencies to help deliver outcomes of collective benefit. In parallel, there has been a large increase in the amount and quality of the research evidence available on behavioural public policy. This review takes two contrasting areas where behavioural insights have been used: tax collection where government policy is compulsory (i.e. requiring compliance), and energy use where social objectives are non-compulsory, and achieved more by persuasion and encouragement. Processes of modifying and changing behaviour require different approaches whether the change is deemed necessary by the state or not. In taxes, the sole use of enforcement is rarely efficacious, whereas increasing the uncertainty of follow-up and audit increases compliance. Offering discounts for energy bills appears to be an effective method for achieving cooperation. However, the use of social norms and increased information and professional advice is effective for both compulsory and non-compulsory areas of compliance and cooperation. This has important implications for policymakers, who may be seeking effective methods of encouraging behaviour change. While there are differences in approaches for compulsory and non-compulsory areas of policy, there may be areas that move from non-statutory to statutory in the future. In this case, the development of desired social norms appears to be the most effective method of ensuring overall compliance.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2126234174</t>
+          <t>https://openalex.org/W3084250059</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4102/ids.v54i2.2579</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Kossoy &amp; Guigon (2012)</t>
+          <t>Jooste &amp; Potgieter (2020)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>State and trends of the carbon market 2012</t>
+          <t>The contested legacy of singing God’s inspired songs in the Reformed Churches in South Africa: The regulating role of the Word from Dordrecht to Totius and into the present</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>The total value of the carbon market grew by 11 percent in 2011, to $176 billion, and transaction volumes reached a new high of 10.3 billion tons of carbon dioxide equivalent (CO2e). This growth took place in the face of economic turbulence, growing long-term oversupply in the EU Emissions Trading Scheme (EU ETS) and plummeting carbon prices. By far, the largest segment of the carbon market was that of EU Allowances (EUAs), valued at $148 billion. With the end of the first commitment period of the Kyoto Protocol in 2012, the value of the pre-2013 primary certified emission reduction (CER), emission reduction unit (ERU) and assigned amount unit (AAU) markets declined in 2011. At the same time, the post-2012 primary Clean Development Mechanism (CDM) market increased by a robust 63 percent, to US$2 billion, despite depressed prices and limited long-term-visibility. Against this backdrop, several new domestic and regional carbon market initiatives gained traction in both developed and developing economies in 2011. Five new jurisdictions (i.e., Australia, California, Quebec, Republic of Korea, and Mexico) passed legislations laying the foundation for cap-and-trade schemes. Together, these initiatives will drive substantial resources towards low-carbon investments and they have the potential to unleash a truly transformational carbon market, in support of a global solution to the climate challenge.</t>
+          <t>This article is a historical–theological inquiry into the Reformed Churches in South Africa (RCSA) and the doctrine behind her historic practice of essentially singing only God’s inspired songs. The catalyst for this investigation is the 2012 RCSA Synod decision to revise Article 69 of the church order – an order based on the one formulated at the 1618–1619 Synod of Dordrecht – to allow for the singing of free hymns. Such a decision marked a significant break with the early Reformed and confessional tradition of singing only God’s inspired songs, as well as a driving reason for the formation of the RCSA in 1859. This article challenges the 2012 revision of the Dort-modelled Article 69 on historical and theological grounds. In addition to failing to reckon adequately with her pre-formation history, the RCSA did not give appropriate attention to her rich legacy of singing predominantly Psalms only. More specifically, this article contends that within her own history the RCSA has a confessional and theological category that can help re-establish continuity with the best of her Reformed liturgical past. This category is the scriptural or regulative principle of worship (S/RPW) – a doctrine that has encouraged the reformation of public worship across the globe and one at least latent in the historical RCSA theological discourse. This essay commends its recovery for the future reformation of worship for the glory of God.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4205650312</t>
+          <t>https://openalex.org/W4390294166</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.nbsj.2022.100009</t>
+          <t>https://doi.org/10.59403/12pan1c</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sowińska-Świerkosz &amp; García (2022)</t>
+          <t>Mazansky (2015)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>What are Nature-based solutions (NBS)? Setting core ideas for concept clarification</t>
+          <t>Hybrid Debt and Hybrid Equity Instruments and the Interest Limitation Rules in South Africa</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Although nature-based solutions (NBS) have been promoted as a key tool for solving diverse environmental and societal problems, the concept and its practical applications remain unclear. This ambiguity is linked to the fact that the NBS concept has emerged from the integration of multiple scientific fields. In addition, there has been a delay in establishing clear standards for NBS, hence a number of actions that today would be seen as complementary or related measures, are frequently branded as NBS. Thus, this paper paves the way to clarify NBS by identifying their core features and formulating criteria to exclude certain actions from the set of NBS. After reviewing 20 definitions of NBS, these actions are identified as interventions that: (1) are inspired and powered by nature; (2) address (societal) challenges or resolve problems; (3) provide multiple services/benefits, including biodiversity gain; and (4) are of high effectiveness and economic efficiency. The non-systematic review includes both peer-review research papers and relevant official reports, enabling the formulation of a set of criteria that exclude green/blue interventions from the set of NBS. These are: (1) lack of functioning ecosystems; (2) random actions; (3) post-implementation goal(s); (4) negative/no impact on biodiversity; (5) same benefits as grey infrastructure alone; (6) unfair distribution of benefits; (7) ‘copy-paste’ implementation approach; (8) top-down model of governance; (9) static management approach; (10) financial expenses disproportionate to benefits; and (11) ‘point scale’ approach. Ongoing and future practice will contribute to our understanding of the long-term operation of NBS as well as to the detection of synergies and trade-offs, thereby enabling us to better define this concept's boundaries.</t>
+          <t>In this article, the author examines the South African tax rules relating to hybrid debt and hybrid equity instruments, particularly with a view either to disallowing deductions or taxing receipts. Some observations are also made on the related interest limitation rules, which prevent excessive interest deductions.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3043004278</t>
+          <t>https://openalex.org/W4229755219</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1002/wcc.670</t>
+          <t>https://doi.org/10.1108/oxan-db262015</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Newell (2020)</t>
+          <t>NA (2021)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>The business of rapid transition</t>
+          <t>Ukraine's campaign against oligarchs rings hollow</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Abstract In a context of climate emergency and calls from the IPCC for “transformative systemic change,” we need to revisit the role of business in helping to accelerate responses to climate crisis. The scale and depth of the challenges facing business have intensified in ways which force us to refocus our research on questions of urgency and speed, as well as the growing need for new and alternative business models and a fundamental re‐balancing of the economy. There is a large literature dealing with business responses to climate change from a range of perspectives and disciplines covering issues such as corporate strategy and public policy engagement. But I argue that the question of the nature and speed of change now required, and whether there are historical and contemporary precedents for accelerated transitions within and beyond business, must assume a more central place in our research. This must be alongside growing efforts to understand how business will adapt to climate chaos. This conclusion implies a closer engagement and cross‐fertilization of ideas with scholars of sustainability transitions, for example. Here, there is growing interest in the question of how to accelerate transitions, but where greater attention is required to the role of business actors. This article is categorized under: The Carbon Economy and Climate Mitigation &amp;gt; Decarbonizing Energy and/or Reducing Demand Policy and Governance &amp;gt; Private Governance of Climate Change</t>
+          <t>Significance Zelensky says the law is not intended to kill off big business but to neutralise corrosive influences on the political system. The law placed before parliament on June 2 requires a list of designated oligarchs to be drawn up, with asset declarations and certain restrictions on what they can do outside their core commercial activities. Impacts The oligarch bill will dominate the domestic agenda over the coming weeks, overshadowing other, often more pressing issues. The law may undergo some amendment, though not necessarily substantive. Foreign lenders will welcome the law without allowing it to be used as an excuse for evading thorough systemic reforms.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4244756598</t>
+          <t>https://openalex.org/W3121379735</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1515/iupac.84.0474</t>
+          <t>https://doi.org/10.1007/bf03546478</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Templeton et al. (2016)</t>
+          <t>Oosterbeek &amp; Patrinos (2009)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Cytolysis, Immune</t>
+          <t>Financing lifelong learning</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>The primary objective of this “Glossary of Terms Used in Immunotoxicology” is to give clear definitions for those who contribute to studies relevant to immunotoxicology but are not themselves immunologists. This applies especially to chemists who need to understand the literature of immunology without recourse to a multiplicity of other glossaries or dictionaries. The glossary includes terms related to basic and clinical immunology insofar as they are necessary for a self-contained document, and particularly terms related to diagnosing, measuring, and understanding effects of substances on the immune system. The glossary consists of about 1200 terms as primary alphabetical entries, and Annexes of common abbreviations, examples of chemicals with known effects on the immune system, autoantibodies in autoimmune disease, and therapeutic agents used in autoimmune disease and cancer. The authors hope that among the groups who will find this glossary helpful, in addition to chemists, are toxicologists, pharmacologists, medical practitioners, risk assessors, and regulatory authorities. In particular, it should facilitate the worldwide use of chemistry in relation to occupational and environmental risk assessment.</t>
+          <t>This paper describes and analyzes different financial schemes to promote lifelong learning. Positive effects of financial incentives to pupils are not restricted to high ability pupils, as low ability students also seem to benefit. The evidence regarding the effects of subsidy forms is limited. The most prominent knowledge gaps regarding the effects of various financing schemes related to lifelong learning are the effects of vouchers; financial aid schemes for students; and entitlements and individual learning accounts.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4386742978</t>
+          <t>https://openalex.org/W1974416061</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1007/s12155-023-10671-x</t>
+          <t>https://doi.org/10.1016/j.radphyschem.2005.04.019</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Mohammadi et al. (2023)</t>
+          <t>Wojnárovits et al. (2005)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Energy Production Features of Miscanthus Pellets Blended with Pine Sawdust</t>
+          <t>Reactivity differences of hydroxyl radicals and hydrated electrons in destructing azo dyes</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Abstract The primary objective of this study was to evaluate the qualities of Miscanthus pellets blended with pine sawdust at various ratios ( Miscanthus /pine sawdust—0:100, 25:75, 50:50, 75:25, and 100:0) and relate them to energy generation potential under typical production conditions of the widely used bioenergy production technologies according to literature. Samples of each material were milled to the required sizes and blended in the proportions mentioned above. Water was added (6%) to each mixture to achieve a uniform moisture content of 10% on wet basis. The mixtures were then subjected to pressure agglomeration in the form of mechanical compression using a single pellet press so that homogeneously sized fuel pellets were obtained. Thereafter, the pure and blended pellet samples were examined using a range of analytical techniques to reveal any alterations in characteristics important to the utilization of the pellets as a green energy source. The results showed that, although temperature variations generally caused an estimated 6% moisture loss on a wet basis during pelleting with positive influence on the features of the pellets, the quality of the pellets in terms of ash composition (2–4%), hardness (41–46 kg/pellet), and heating value (20–21 MJ/kg) was in general more desirable for the blended pellets than for pure Miscanthus pellet. Structural analysis also revealed low levels of hydrophobic groups in the blends relative to pure Miscanthus , which were consistent with the fractions of pine sawdust and were also the reason for the pellets’ increased hardness.</t>
+          <t>The high-energy radiation-induced degradation of an H-acid derivative azo dye, Apollofix-Red SF-28 (AR-28) was studied in aqueous solution by using pulse radiolysis with kinetic spectroscopic detection for transient measurements. Gamma radiolysis with UV-VIS spectroscopy and gradient ionpair HPLC separation with diode array detection were applied for following the destruction of AR-28 and measuring the products. The reactions of hydrated electron (eaq−) and hydroxyl (OH) radical were investigated separately. OH reacts with the unsaturated bonds of the molecule. In the further reactions of the OH adduct radicals, the AR-28 molecules partly reform with a slightly modified structure. The products formed in the first reaction of OH and AR-28 molecules have also high reactivity towards the OH radicals. For these reasons the efficiency of OH radicals in discolouration of the solution is relatively low, it is below 0.5. The efficiency is much higher, close to unity for eaq−. The reaction of eaq− with AR-28 leads to an immediate destruction of the colour-giving centre.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4365394989</t>
+          <t>https://openalex.org/W568585734</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1137/1.9781611977653.ch108</t>
+          <t>https://doi.org/10.22440/econworld.j.2015.1.1.sk.0004</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Yang et al. (2023)</t>
+          <t>Koç &amp; Erkin (2015)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Data Mining Challenges and Opportunities to Achieve Net Zero Carbon Emissions: Focus on Electrified Vehicles</t>
+          <t>Standards, Inequality in Education and Efficiency</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Society must achieve net zero carbon emissions to mitigate anthropogenic climate change and preserve a livable planet. Reducing transportation emissions is an important component to achieve net zero because such emissions account for a quarter of global carbon released into the environment. Driven by increasingly available transportation big data and enhanced computational speed, data mining techniques have become powerful tools to achieve transportation decarbonization. This paper describes existing gaps in transportation decarbonization research where data mining can help address problems related to medium and heavy vehicle electrification, electric micromobility safety, and analysis of alternative fuel-powered and plug-in hybrid electric vehicles. Our recommendations encompass open research problems, opportunities for data mining applications, and examples of areas where advancements in data mining techniques are needed. We encourage the data mining community to explore these challenges and opportunities to help achieve net zero emissions goals.</t>
+          <t>We develop a model of educational standards that includes inequality in educational opportunities. Our model shows that policymakers setting an output maximizing standard need to consider structural factors such as inequality of income and opportunity, skill mismatch in the economy, profit and wage shares and labor market imperfections. High standards are not optimal under severe educational inequality; they lead to lower output when many cannot access quality education. Optimal standard rises along with increasing opportunities for poor students. Targeted subsidies enhance both distributional and efficiency-related objectives. Other effective policies to extend skilled labor and to improve poor workers income are remedying information problems between employers and workers and distributing more of output gains toward labor.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4308127043</t>
+          <t>https://openalex.org/W3212788577</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://doi.org/10.3390/su142114268</t>
+          <t>https://doi.org/10.1515/jgd-2021-0052</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Shabangu et al. (2022)</t>
+          <t>Kose et al. (2022)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Microbial Fuel Cells for Electrical Energy: Outlook on Scaling-Up and Application Possibilities towards South African Energy Grid</t>
+          <t>A Mountain of Debt: Navigating the Legacy of the Pandemic</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Microbial fuel cell (MFC) technology turns chemical energy into bioelectricity in a clean and efficient manner, lowering carbon emissions and increasing bioenergy production. It is a multifaceted technique that has the potential to be a panacea for clean water scarcity and sustainable, renewable energy. In this review, the approach focuses on scaling-up and application prospects at a commercial scale. An outlook on various, previously tried methodologies was generated in order to establish a viable bioelectricity scaling-up approach that is also cost-effective in its design. Precise themes were followed to evaluate previously produced models and methodologies for MFCs: principle and anatomical mechanisms, basic applications, bioelectricity scaling-up potentials from previous work and limitations, then an outlook on MFC feasibility and its wastewater treatment plant (WWTP) energy supply chain. The goal of this paper is to derive a viable approach from prior research in order to comprehend how MFC technology may be scaled-up for commercial and practical power output. Essentially, this article summarizes the current energy predicaments faced by South Africa and proposes MFCs as a new knowledge-contributing technology with electricity scaling-up potential. Conclusively, more research on MFC technique scaling-up operating factors is recommended.</t>
+          <t>Abstract The COVID-19 pandemic has triggered a massive increase in global debt levels and exacerbated the trade-offs between the benefits and costs of accumulating government debt. This paper examines these trade-offs by putting the recent debt boom into a historical context. It reports three major findings. First, during the 2020 global recession, both global government and private debt levels rose to record highs, and at their fastest single-year pace, in five decades. Second, the debt-financed, massive fiscal support programs implemented during the pandemic supported activity and illustrated the benefits of accumulating debt. However, as the recovery gains traction, the balance of benefits and costs of debt accumulation could increasingly tilt toward costs. Third, more than two-thirds of emerging market and developing economies are currently in government debt booms. On average, the current booms have already lasted three years longer, and are accompanied by a considerably larger fiscal deterioration, than earlier booms. About half of the earlier debt booms were associated with financial crises in emerging market and developing economies.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4296986775</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1108/jbs-03-2022-0048</t>
+          <t>https://openalex.org/W3122454879</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Jackson &amp; Hodgkinson (2022)</t>
+          <t>Immordino &amp; Russo (2016)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Keeping a lower profile: how firms can reduce their digital carbon footprints</t>
+          <t>Cashless Payments and Tax Evasion</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Purpose In the pursuit of net-zero, the decarbonization activities of organizations are a critical feature of any sustainability strategy. However, government policy and recent technological innovations do not address the digital carbon footprint of organizations. The paper aims to present the concept of single-use dark data and how knowledge reuse by organizations is a means to digital decarbonization. Design/methodology/approach Businesses in all sectors must contribute to reducing digital carbon emissions globally, and to the best of the authors’ knowledge, this paper is the first to examine “how” from a knowledge (re)use perspective. Drawing on insights from the knowledge creation process, the paper presents a set of pathways to greater knowledge reuse for the reduction of organizations’ digital carbon footprint. Findings Businesses continually collect, process and store knowledge but generally fail to reuse these knowledge assets – referred to as dark data. Consequently, this dark data has a huge impact on energy use and global emissions. This model is the first to show explicit pathways that businesses can follow to sustainable knowledge practices. Practical implications If businesses are to be proactive in their collective pursuit of net-zero, then it becomes paramount that reducing the digital carbon footprint becomes a key sustainability target. The paper presents how this might be accomplished, offering practical and actionable guidance to businesses for digital decarbonization. Originality/value Two critical questions are facing businesses: how can decarbonization be achieved? And can it be achieved at a low-cost? Awareness of the damaging impact digitalization may be having on the environment is in its infancy, yet knowledge reuse is a proactive and cost-effective route to reduce carbon emissions, which is explored in the paper.</t>
+          <t>Cashless payments hinder tax evasion because they build a trail for the underlying transactions. We find empirical evidence supporting this claim for Europe, showing a negative relationship between VAT evasion and the payments with credit and debit cards. We also find that using electronic cards to gather cash at ATMs, by making cash more abundant, fosters VAT evasion. Policies aimed at reducing tax evasion should therefore subsidize the direct use of electronic cards as payments, not their possession.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4391789259</t>
+          <t>https://openalex.org/W3122309441</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://doi.org/10.2139/ssrn.4723862</t>
+          <t>https://doi.org/10.2139/ssrn.3079256</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Powae &amp; Rao (2024)</t>
+          <t>Eroglu &amp; Zehra (2017)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Quantification of Soil Nutrient Stocks and Stoichiometric Ratios in Eucalyptus Pellita Biomass Plantation Chronosequence in Papua New Guinea</t>
+          <t>The Political Economy of International Standard Setting in Financial Reporting: How the United States Led the Adoption of IFRS Across the World</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Eucalyptus pellita biomass tree plantations have been extensively established for bioenergy generation and carbon capture in the native grasslands of Markham Valley in Papua New Guinea. The consequences of land use conversion from grasslands to energy plantations and the changes in the soils of the chronosequence of bioenergy plantation are least explored. This study evaluated dynamic changes in key soil physico-chemical properties, nutrient stocks of soil organic carbon (SOC), nitrogen (TN) and phosphorus (TP), and their stoichiometric ratios in a plantation chronosequence comprising 2-, 4-, 7- and 10-year-old tree stands, paired with native grasslands at two sampling intervals (January and June). The soil NH4+-N concentration declined with the age of the biomass plantations compared with steady levels of NO3—N in the chrono sequence. The SOC and TP concentration and stocks were significantly (p &lt; 0.05) impacted by the age of Eucalyptus tree stands but not TN. The SOC and TP stocks in the top 45 cm of the chronosequence soil depleted at the rates of 0.19 Mg ha-1y-1and 0.011 Mg ha-1 y-1, respectively. The wider stoichiometric ratio of C:N (&gt; 25:1) in soils of 4- and 7-year plantations showed possible immobilization and deficiency of mineral N to meet the nutrition of trees. The C:P ratios in the chronosequence were &lt;200 favoring net mineralization of organic P compounds. Afforestation of grasslands with E. pellita biomass plantation is not ecologically beneficial, considering solely the belowground SOC sequestration potential.</t>
+          <t>Historically, every country had its own accounting standards, each merging to some extent with its local corporate, labor, and tax laws. No matter how undesirable, it was natural to expect differences among nations. Globalization made these differences so impractical that from corporate leaders to accountants to government officials, many pushed for harmonized accounting standards. _x000D_
+_x000D_
+Pursuing this goal, a private international organization was created to set standards for the world. Currently around 120 countries require or permit International Financial Reporting Standards (IFRS), however, the United States is yet to make a decision to adopt these international standards._x000D_
+_x000D_
+The adoption of IFRS in the United States would, in theory, be easier compared to the experience of the European Union. The EU mandated that all publicly traded firms use IFRS in their consolidated financial statements from 2005 onwards. Several issues are yet to be resolved, but Europe managed to achieve what was once thought to be an insuperable task in coordinating a common standard for its Member States. _x000D_
+_x000D_
+If the adoption of IFRS in the United States would be easier than the EU experience, why has the United States not adopted IFRS? With this paper, I argue that IFRS are a set of U.S. supported Anglo-American accounting standards. Further, that the reason for creating IFRS was not necessarily for the United States to adopt them but to convert the patchwork of accounting standards around the world into a single system that is similar to U.S. GAAP.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1509563301</t>
+          <t>https://openalex.org/W4244048923</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/b978-0-08-030580-6.50014-0</t>
+          <t>https://doi.org/10.1002/9781119176695.ch17</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Lewis (1984)</t>
+          <t>Glassie (2016)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Appropriate Biotechnology for Rural Communities in the Developing Countries</t>
+          <t>Legal Considerations</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>The continued importance of the rural sectors, and particularly agriculture, to the economies of the world's developing countries is demonstrated. However, there are shortages of available energy in Third World rural communities, which can be alleviated by the utilisation of various biotechnologies and bioenergy production and conservation techniques, to increase both agricultural potential and quality of life. It is shown how energy self-reliance can be achieved using such technologies in a case study of a southern Indian village, employing a systems analysis methodology to ascertain the outcome of a plausible technocratic scenario. This kind of approach can then be used to assess the feasibility of food and fuel self-reliance in other communities existing under various conditions throughout the developing world.</t>
+          <t>Membership associations must have the trust and confidence of their members, constituencies, and the public to operate successfully. This chapter covers some important legal issues related to membership, including corporate, tax exemption, antitrust, due process, and intellectual property. The board of directors of an association has the ultimate authority to manage the association, including usually setting dues for members and approving the budget. The board also usually has the right to discipline members, including terminate members for bad conduct or violation of law or a code of ethics. In addition to antitrust claims by individuals who may be denied membership or those whose membership is revoked, legal challenges can be brought by such persons on the basis of common law fairness principles, generally referred to as due process. The Internet has transformed the communications among association members and stakeholders. There are legal risks associated with electronic communications and social media.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2408271229</t>
+          <t>https://openalex.org/W2234790633</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Schroeder et al. (2014)</t>
+          <t>Verčič &amp; Verčić (2014)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Testing alternative response designs for training forest disturbance and attribution models</t>
+          <t>Reflexive mediatization and remaking of the middleman</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Understanding and modeling land cover and land use change is evolving into a foundational element of climate, environmental, and sustainability science. Land cover and land use data are core to applications such as carbon accounting, greenhouse gas emissions reporting, biomass and bioenergy assessments, hydrologic function assessments, fire and fuels planning and management, and forest and rangeland health assessments. Remote sensing-based monitoring efforts like the North American Forest Dynamics (NAFD) project, and the newly launched Landscape Change Monitoring System (LCMS), will provide land cover and land use change data on all U.S. lands for the longest possible historical period. Empirical models driving disturbance and causal maps rely on large quantities of high quality data. Many decisions need to be made about the size, shape, quantity, quality, and other details about the training plots themselves, i.e., the response design. Here, the authors explored best practices for collecting training data for these empirical models on 10 pilot scenes in the United States. Alternative designs were evaluated in terms of their costs and benefits for national mapping applications.</t>
+          <t>The emergence of public relations in early 20th century was largely fuelled by the rapid mediatization of society. As journalists gained power as middlemen between organizations and society framing news and setting public agenda in the mass media, organizations (corporations and governments alike) responded by introducing counter-parts on their side: public relations practitioners as middlemen between the mass media and organizations. Public relations practitioners enabled organizations to become reflexive (van Ruler and Vercic 2005) to the mass media expectations and adjust their behaviors to journalistic needs. Media relations -- management of relations between organizations and the mass media -- is the most common practice area in the public relations sector (Swerling, Thorson &amp; Tenderich 2012 ; Wilson &amp; Supa 2013 ; Zerfass et al. 2011). In the second half of the 20th century, more than 150 studies explored relations between public relations and the mass media and they found that between 20 and 80 per cent of the journalistic media content was influenced by some sort of ‘information subsidies’ provided by public relations (Cameron, Sallot &amp; Curtin 1997). But that was when journalism as a profession was on its peak and public relations was only becoming an aspiring profession. Sullivan (2011) collected data on changes in the relative weights of the two sides. In the past 30 years, the number of journalists per 100, 000 Americans dropped from .36 to .25. At the same time, the number of public relations practitioners per 100, 000 Americans rose from .45 to .90. Now there are more than three public relations practitioners per one journalist. Between 2000 and 2009, the newspaper advertising revenue in the US dropped from $49 to $22 billion. Between 1997 and 2007 revenues of the US public relations agencies went up from $43.5 to $8.75 billion. The number of US newspaper reporters and editors dropped from 56, 900 in 1990 to 41, 600 in 2011. The number of people employed by the US public relations agencies increased from 38, 735 in 1997 to 50, 499 in 2007. While introduction of public relations practitioners since 1920s lead to reflexivity in media relations, what is emerging today leads to a new phenomenon of reflexive mediatization: non-core-media organizations (corporations and government agencies) are reflexively mediatizing themselves. From providers of information subsidies, public relations is transforming into media producer and distributor of stories and news. Coca-Cola corporation is experimenting with its own “brand journalism” in its digital magazine - http://www.coca-colacompany. com (Working 2013). In September 2013, Alex Aiken, the Executive Director of the UK Government Communications declared: “The press release is dead.” (Magee 2013). In January 2014, Kim McKinnon, the Canadian Government’s Communications Community officer, published the following statement on the Canadian Government official website: “The Government of Canada is retiring the traditional press release format in favour of a more digital-friendly product that makes the key messages of announcements clearer, quick facts more accessible and integrates more effectively with social media channels.” (McKinnon 2014). The paper introduces the notion of reflexive mediatization and proposes conceptual apparatus to tackle with it.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1509597683</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.22004/ag.econ.124311</t>
+          <t>https://openalex.org/W2295180544</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Gowen et al. (2012)</t>
+          <t>陳寀囷 (2006)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>A bioeconomic model of carbon trading within an Australian grazing enterprise</t>
+          <t>以資源基礎理論探討『永信藥品』國際化策略</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>The Carbon Farming Initiative (CFI) and other carbon trading programs have been promoted as alternative sources of income for agricultural producers, particularly those on marginal land. This paper presents the results of a bioeconomic model developed to compare the relative returns from a beef enterprise against changing regrowth management practices to sequester additional carbon and sell carbon offsets. The model is constructed based on a 1000 hectare parcel of land in Central Queensland and is calculated for two landtypes; Brigalow and Eucalypt. Assuming zero transaction costs and a 20 year contract period, a carbon-cattle enterprise has higher returns that a cattle-only enterprise at relatively low carbon prices for both land types. However, results are highly dependent on the underlying assumptions regarding transaction costs, previous clearing methods and opportunity costs of cattle production. The impact of these variables and alternative policy settings were evaluated using an optimization model which identifies the optimal allocation between the two enterprises at different carbon prices. Whilst the model indicates that some beef producers could increase returns by supplying carbon offsets, the results are highly variable and do not account for the risk and uncertainty associated with long term contracts to supply a non-market good into a new market.</t>
+          <t>The coming of globalization, pharmaceutical industry not only has to encounter the change of outer environment, but also has to promote managerial ability to deal with the distribution of resources inside the organization to cope with all kinds of operating crisis and risk raised by the encountering of globalizing competitive environment. In the need of society, Taiwan is facing a trend of downsizing birth rate and an increasing aging population gradually in the recent years, which also brings up the need for medicine and care. To the pharmaceutical industry, it is believed that the national market can not reach the scaled economy. In addition, the technology can not be effectively improved and so it is difficult to open oversea markets. Furthermore, the practice of health and care regulations such as medicine pricing standard, medicine classification, separation of clinic and pharmacy and so on, causes a reform of pharmaceutical market and brings a great shock to the industry. The study is based on the Resource-Based Theory, and making an observation to the leader of pharmaceutical industry –Yung Shin Pharmaceutical on how Yung Shin Pharmaceutical can breakthrough the encountering of the competition between the foreign invested pharmaceutical facilities and national pharmaceutical facilities, and still maintain the leading position in the industry, as well, is capable of using the globalizing strategy to setup subsidiaries in Malaysia, States and China. For Malaysia is the first base oversea for A company, the study also emphasizes on the analysis of Yung Shin Pharmaceutical on the decision making of subsidiary setup in Malaysia, to discuss the strategic choice and resource application for an organization in order to achieve the expected growth and extension, and to ensure the development and correct direction of the industry. Then hope to understand the identification and operation of the critical resource in an organization, to further discussion of the moving on into global market by taking the competitive advantage of extensive resources.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4310875080</t>
+          <t>https://openalex.org/W3138760678</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.apenergy.2022.120452</t>
+          <t>https://doi.org/10.1086/ntj41790717</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Li et al. (2023)</t>
+          <t>Holzman (1958)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Forecasting carbon prices based on real-time decomposition and causal temporal convolutional networks</t>
+          <t>INCOME TAXATION IN THE SOVIET UNION: A COMPARATIVE VIEW</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Recently, global attention has been paid to climate change. On this account, the market-based carbon pricing scheme is developed to limit greenhouse gas emissions, where a proper grasp of the pricing mechanism is crucial for alleviating global warming. Accordingly, we propose a novel method to interpret carbon price dynamics, concurrently deriving the precise prediction and causality. Due to the nonlinearity and nonstationarity of carbon prices, we develop a real-time decomposition approach coupling the multiple ensemble patch transform (MEPT) and the improved complete ensemble empirical mode decomposition with adaptive noise (ICEEMDAN). The MEPT captures the multi-resolution trends of the carbon prices series exactly, and then the ICEEMDAN extracts the fluctuation patterns. Additionally, we collect the numerous potential factors, involving energy sources, energy prices, stock market indices, and economic information. Furthermore, we developed causal temporal convolutional networks (CTCNs) to realize the accurate prediction and the proper causal inference simultaneously. The experimental results on the European Union Allowance (EUA) confirm the effectiveness and necessity of the real-time MEPT-ICEEMDAN decomposition. Moreover, the proposed MEPT-ICEEMDAN-CTCN model exhibits significant superiority in multi-step-ahead and quantile forecast, which realizes the 0.73881%, 1.04461%, and 1.23495% MAPE in one-, five-, and ten-step-ahead forecast respectively and 0.00032 PDQ0.1 and the 0.00285 PDQ0.9 in the quantile forecast. Meanwhile, it reveals the nonlinear Granger causality across the various horizons and quantiles for the first time. It is instructive and inspiring for policymakers, carbon-consumed industries, investors, and researchers.</t>
+          <t>Next article No AccessINCOME TAXATION IN THE SOVIET UNION: A COMPARATIVE VIEWFRANKLYN D. HOLZMANFRANKLYN D. HOLZMAN Search for more articles by this author PDFPDF PLUS Add to favoritesDownload CitationTrack CitationsPermissionsReprints Share onFacebookTwitterLinkedInRedditEmail SectionsMoreDetailsFiguresReferencesCited by National Tax Journal Volume 11, Number 2June 1958 Published for: The National Tax Association Article DOIhttps://doi.org/10.1086/NTJ41790717 Views: 5Total views on this site Citations: 1Citations are reported from Crossref © 1958 National Tax Association. All rights reserved.PDF download Crossref reports the following articles citing this article: Yanni Kotsonis “No Place to Go”: Taxation and State Transformation in Late Imperial and Early Soviet Russia Kotsonis, The Journal of Modern History 76, no.33 (Jul 2015): 531–577.https://doi.org/10.1086/425440</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4235345770</t>
+          <t>https://openalex.org/W4251178260</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1515/iupac.87.0203</t>
+          <t>https://doi.org/10.1093/he/9780198848455.003.0006</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Templeton et al. (2016)</t>
+          <t>Dignam &amp; Lowry (2020)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Dysaphia</t>
+          <t>6. Raising capital: debentures: fixed and floating charges</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>The primary objective of this Glossary of Terms Used in Neurotoxicology is to give clear definitions for those who contribute to studies relevant to neurotoxicology, or must interpret them, but are not themselves neurotoxicologists, neuroscientists or physicians. This applies especially to chemists who need to understand the literature of neurotoxic effects of substances without recourse to a multiplicity of other glossaries or dictionaries. The Glossary includes terms related to basic and clinical neurology insofar as they are necessary for a self-contained document, and particularly terms related to diagnosing, measuring, and understanding effects of substances on the central and peripheral nervous systems. The glossary consists of about 800 terms as primary alphabetical entries, and includes Annexes of common abbreviations, and examples of chemicals with known effects on the nervous system. The authors hope that among the groups who will find this glossary helpful, in addition to chemists, are toxicologists, pharmacologists, medical practitioners, risk assessors, and regulatory authorities. In particular, it should facilitate the worldwide use of chemistry in relation to occupational and environmental risk assessment.</t>
+          <t>Titles in the Core Text series take the reader straight to the heart of the subject, providing focused, concise, and reliable guides for students at all levels. This chapter discusses corporate borrowing through debentures or debenture stock, as well as fixed and floating charges that companies issue to creditors as security interests. It begins by outlining some important distinctions between the ability of small and large companies to raise loan capital. It then considers the priority of secured creditors and the registration requirements for charges, the issue of whether or not a fixed charge could be created over a company’s book debts, provisions for automatic crystallisation that converts the floating charge into an equitable fixed charge over company assets, and reform of security interests.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4385740986</t>
+          <t>https://openalex.org/W2033239264</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://doi.org/10.3390/en16165911</t>
+          <t>https://doi.org/10.1111/j.1759-5436.1978.mp9004009.x</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Kowalski et al. (2023)</t>
+          <t>Portes (1978)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Improving the Quality of Hydroxyapatite Ashes from the Combustion of Meat-Bone Meal in an Industrial Rotary Kiln</t>
+          <t>The Informal Sector and the World Economy: Notes on the Structure of Subsidised Labour</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Research on the properties of hydroxyapatite ashes from an industrial unit burning meat and bone meal in an industrial rotary kiln is presented. High carbon content (10%), relatively low phosphorus (34%), and sulfides were found. The ash obtained was unsuitable for producing superphosphate fertilizer due to the emission of hydrogen sulfide in the reaction of the raw material with sulfuric acid. The research showed that decreasing the meat-bone meal calcining temperature below 950 °C and recycling the ashes, reusing them after mixing in a 1:1 ratio with dosed meat and bone meal, allows reducing the carbon content in the hydroxyapatite ash to the level of &amp;lt;0.2%, increases the P2O5 content in the ash to 39%, and eliminates hydrogen sulfide emissions. The improved parameters allow the production of hydroxyapatite ash that could be a substitute for phosphorites used in the production of fertilizers. Incineration of the meat-bone meal allowed the production of bioenergy and hydroxyapatite. This is an example of implementing a very profitable circular economy solution.</t>
+          <t>SUMMARY The informal sector in Third World cities was initially identified as the mechanism by which the poor managed to survive under adverse conditions. Subsequent studies showed how interdependent informal activities were with those in the formal sector. Most studies interpreted this as evidence of the dependent and interstitial character of the informal economy. This paper argues that, from the point of view of structural arrangements, the opposite is more accurate. The informal sector provides a subsidy to formal sector consumption and cheapens labour costs directly when used in a ‘contract’ capacity by formal enterprises. RESUMEN El sector informal y la economia mundial : anotaciones en torno a la estructura de la mano de obra subvencionada El sector informal de las ciudades del tercer mundo se identifico en un principio como el mecanismo por el que lo pobre conseguían sobrevivir en condiciones adversas. Estudios posteriores mostraron la gran interdependencia entre las actividades informales y las del sector formal. Casi todos los estudios interpretaron este fenómeno como una prueba del carácter estrechamente dependiente de la economía informal. Este artículo se propone probar que, desde el punto de los elementos estructurales, lo contrario es más exacto. El sector informal ofrece una subvención al consumo del sector formal y abarata directamente los costes de la mano de obra cuando ésta se utiliza en una capacidad de “contrato” por parte de las empresas formales. RESUME Le secteur non‐officiel et l'économie mondiale: remarques sur la structure de la main‐d'oeuvre subventionnée Le secteur non officiel dans les villes du Tiers Monde était identifié initialement comme le mécanisme par lequel les pauvres parviennent à survivre dans des conditions adverses. Par la suite, des études ont montré comment des activités non officielles étaient inter‐dépendantes avec celles du secteur officiel. La plupart des études interprétaient ceci comme l'évidence du caractère dépendant et interstitiel de l'économie non officielle. L'auteur affirme que, du point de vue des arrangements structurels, le contraire est plus exact. Le secteur non officiel fournit une subvention à la consommation du secteur officiel et abaisse le coût de la main‐d'oeuvre directement lorsque des entreprises formelles y ont recours pour des travaux à facon.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2034084499</t>
+          <t>https://openalex.org/W1913441637</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.envsoft.2015.03.014</t>
+          <t>https://doi.org/10.1007/s40815-015-0067-7</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Smajgl et al. (2015)</t>
+          <t>Kabak et al. (2015)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Assessing the effectiveness of payments for ecosystem services for diversifying rubber in Yunnan, China</t>
+          <t>Critical Success Factors for the Iron and Steel Industry in Turkey: A Fuzzy DEMATEL Approach</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Monoculture rubber plantations are rapidly expanding throughout Southeast Asia. The Prefecture of Xishuangbanna is characterised as both an epicenter of Chinese biodiversity and rubber production. The rapid conversion of native primary forest into rubber plantations has introduced tensions between the competing political goals to conserve biodiversity and heritage landscapes – both driving the rapidly emerging tourism industry – and economic aspirations at household and district levels. In China, decision makers discuss payments for ecosystem service schemes to resolve these tensions. As a component of the policy development process, this research project was invited to inform the political debate. Agent-based simulations revealed perverse outcomes of payments for ecosystem services, intended to encourage the conversion of monoculture rubber into agroforestry rubber. As an outcome of this modelling-based initiative, managing agencies have revised previously drafted payment schemes and reconsidered the importance of monitoring and regulatory approaches.</t>
+          <t>The attempt to improve the efficiency and competitiveness of an industrial sector is aided by the determination of critical success factors (CSFs) which focus efforts in those areas that really affect the whole industry, thereby conserving limited resources. In this paper, a three-stage methodology is proposed to find CSFs for an industrial sector. The methodology specifies the interrelations between factors that shape the global competitiveness of a country as a whole and those that shape the competitiveness of the particular industry in question. It integrates a Web-based survey, a Delphi-type workshop, and a fuzzy decision making trial and evaluation laboratory model to highlight those CSFs upon which policymakers should especially concentrate in order to increase the competitiveness of a given industry. This methodology is then applied to a case study, identifying the CSFs of the iron and steel industry in Turkey. The results show that the burden of custom procedures, total tax rate, scope and impact of taxation, and solidity of banks are the CSFs for the competitiveness of the Turkish iron and steel industry.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1991521713</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/s0269-7491(01)00220-2</t>
+          <t>https://openalex.org/W3122937310</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Eve et al. (2002)</t>
+          <t>Busch &amp; Mukherjee (2017)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>National-scale estimation of changes in soil carbon stocks on agricultural lands</t>
+          <t>Encouraging State Governments to Protect and Restore Forests Using Ecological Fiscal Transfers: India’s Tax Revenue Distribution Reform</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Average annual net change in soil carbon stocks under past and current management is needed as part of national reporting of greenhouse gas emissions and to evaluate the potential for soils as sinks to mitigate increasing atmospheric CO2. We estimated net soil C stock changes for US agricultural soils during the period from 1982 to 1997 using the IPCC (Intergovernmental Panel on Climate Change) method for greenhouse gas inventories. Land use data from the NRI (National Resources Inventory; USDA-NRCS) were used as input along with ancillary data sets on climate, soils, and agricultural management. Our results show that, overall, changes in land use and agricultural management have resulted in a net gain of 21.2 MMT C year−1 in US agricultural soils during this period. Cropped lands account for 15.1 MMT C year−1, while grazing land soil C increased 6.1 MMT C year−1. The land use and management changes that have contributed the most to increasing soil C during this period are (1) adoption of conservation tillage practices on cropland, (2) enrollment of cropland in the Conservation Reserve Program, and (3) cropping intensification that has resulted in reduced use of bare fallow.</t>
+          <t>In February 2014, India’s 14th Finance Commission added forest cover to the formula that determines the amount of tax revenue the central government distributes annually to each of India’s 29 states. The Government of India estimates that from 2015–2019 it will distribute $6.9–12 billion per year to states in proportion to their 2013 forest cover, amounting to around $174–303 per hectare of forest per year. Assuming that contemporary forest cover will remain an element of the formula beyond 2020, Indian states now have a sizeable new fiscal incentive to protect and restore forests, contributing to the achievement of India’s climate goals. India’s tax revenue distribution reform creates the world’s first ecological fiscal transfers (EFTs) for forest cover, and a potential model for other countries. In this paper we discuss the origin of India’s EFTs and their potential effects. In a simple preliminary analysis, we do not yet observe that the EFTs have increased forest cover across states, consistent with our hypothesis that one to two years of operation is too soon for the reform to have had an effect. This means there remains substantial scope for state governments to protect and restore forests as an investment in future state revenues.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2357981716</t>
+          <t>https://openalex.org/W2356946553</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Meng (2009)</t>
+          <t>Wang (2004)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>The reliability of groundwater exploitation and the stochastic simulation model of triangular fuzzy numbers coupled</t>
+          <t>Reformation and Innovation of Practical Teaching in Application Oriented Undergraduate Courses</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>During the calculation to the safe yield of groundwater,there is some uncertainty factors that directly affect the accuracy of calculation result.This paper discussed the theory of using triangular fuzzy numbers to describe and process the randomness and the fuzziness which impact the amount of groundwater mining.The definite way to bring about the uncertain nature of the incomplete and the accuracy of the data and the information about the groundwater extraction are also discussed.Monte Carlo methods have been used to simulate the triangular fuzzy numbers,by this way the calculation between the triangular fuzzy numbers and its functions can be transformed to the operation between the ordinary real numbers,on this basis building a model of random simulation to the water environmental risk assessment and the triangular fuzzy numbers coupling model(SS-TFN).The results of the risk analysis are more fitted the reality demands than the traditional hydrogeology method.This provide a practical approach to make certain more rational and reliable the amount land of water source to allow mine in the evaluation of groundwater resources in the future work,it can also reduces the related decision-making errors about the groundwater mining to the minimum.</t>
+          <t>Practice-oriented teaching is a very important part of teaching in engineering university especially in application-oriented engineering university and it has an unsubstitutable function in cultivating students' creating sense, spirit and ability. In order to strengthen the reform and innovation of practicing teaching, an independent practicing teaching system must be set up. The system should adjust the practicing teaching contents, reform practicing teaching pattern, coordinate practicing teaching administrating system, establish a scientific and reasonable practicing teaching evaluation system and quality ensuring system.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1929113992</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1111/gcbb.12302</t>
+          <t>https://openalex.org/W3147030200</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Townsend et al. (2016)</t>
+          <t>Weinreich (2013)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Food and bioenergy: reviewing the potential of dual‐purpose wheat crops</t>
+          <t>Fair tax evasion and majority voting over redistributive taxation</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Abstract Within the bioenergy debate, the ‘food vs. fuel’ controversy quickly replaced enthusiasm for biofuels derived from first‐generation feedstocks. Second‐generation biofuels offer an opportunity to produce fuels from dedicated energy crops, waste materials or coproducts such as cereal straw. Wheat represents one of the most widely grown arable crops around the world, with wheat straw, a potential source of biofuel feedstock. Wheat straw currently has limited economic value; hence, wheat cultivars have been bred for increased grain yield; however, with the development of second‐generation biofuel production, utilization of straw biomass provides the potential for ‘food and fuel’. Reviewing the evidence for the development of dual‐purpose wheat cultivars optimized for food grain and straw biomass production, we present a holistic assessment of a potential ideotype for a dual‐purpose cultivar ( DPC ). An ideal DPC would be characterized by high grain and straw yields, high straw digestibility (i.e. biofuel yield potential) and good lodging resistance. Considerable variation in these traits exists among current wheat cultivars, facilitating the selection of improved individual traits; however, increasing straw yield and digestibility could potentially have negative trade‐off impacts on grain yield and lodging resistance, reducing the feasibility of a single ideotype. Adoption of alternative management practices could potentially increase straw yield and digestibility, albeit these practices are also associated with potential trade‐offs among cultivar traits. Benefits from using DPC s include reduced logistics costs along the biofuel feedstock supply chain, but practical barriers to differential pricing for straw digestibility traits are likely to reduce the financial incentive to farmers for growing higher ‘biofuel‐quality’ straw cultivars. Further research is required to explore the relationships among the ideotype traits to quantify potential DPC benefits; this will help to determine whether stakeholders along the bioenergy feedstock supply chain will invest in the development of DPC s that provide food and fuel potential.</t>
+          <t>We shed some light on fairness preferences regarding tax evasion. Individuals perceive income inequality which they are responsible for as fair (e.g. work effort) while inequality resulting from factors outside their reach is regarded as unfair (e.g. productivity or wage rate). This affects the incentives to hide income from tax authorities and supply labor. We set up a model where individuals simultaneously choose unreported income and work effort given a linear taxation scheme. We show the conditions for which individuals respond with lower or higher unreported income and work effort when fair tax evasion is introduced. Beyond, it can be shown that unreported income increases while work effort decreases when the tax rate is raised. Finally, we consider a majority voting over redistributive taxation. Thereby, it is shown that the median voter prefers lower (higher) taxation if she evades less (more) taxes than would be fair since raising the tax rate would enlarge (reduce) the deviation from fair tax evasion. This affects the moral cost as peceived by the individuals.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2768810707</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.3390/bioengineering4040092</t>
+          <t>https://openalex.org/W2364664984</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Soleymani &amp; Rosentrater (2017)</t>
+          <t>Shu-sheng (2008)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Techno-Economic Analysis of Biofuel Production from Macroalgae (Seaweed)</t>
+          <t>The Pedagogical Language and Educational Transformation during the 30 Years of Reform and Opening-up</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>A techno-economic evaluation of bioenergy production from macroalgae was carried out in this study. Six different scenarios were examined for the production of different energy products and by-products. Seaweed was produced either via the longline method or the grid method. Final products of these scenarios were either ethanol from fermentation, or electricity from anaerobic digestion (AD). By-products were digestate for AD, and animal feed, or electricity and digestate, for the fermentation pathway. Bioenergy breakeven selling prices were investigated according to the cost components and the feedstock supply chain, while suggestions for potential optimization of costs were provided. The lowest production level of dry seaweed to meet 0.93 ($/L) for ethanol fuel and 0.07 $/kW-h for electricity was found to be 0.68 and 3.7 million tonnes (dry basis), respectively. At the moment, biofuel production from seaweed has been determined not to be economically feasible, but achieving economic production may be possible by lowering production costs and increasing the area under cultivation.</t>
+          <t>The pedagogy in China experienced rapidest and most fruitful development during 30 years of Reform and Opening-up. In aspect of evolution of academic language, it experienced three phases, namely, phases of of anti-political trend in 1980s, focus and specialization in 1990s, and the cultural pursue beyond knowledge in 2000s.It is also a process in which academic, political and public systems shift from a status of muddy combination to differentiation and independence, then to communication and dialogue and present a of integration. To realize the cultural pursue beyond we should grasp realistic meaning of the unification of theory and practice, unify preciseness of academic theory, increasing knowledge, feeling of humanity, exploration with a characteristic of humanity, and way of expression, so that we can exhibit fully humanity nature of pedagogy.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1988783263</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.renene.2014.03.056</t>
+          <t>https://openalex.org/W2588655847</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>González-Salazar et al. (2014)</t>
+          <t>Fielke (2015)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Methodology for biomass energy potential estimation: Projections of future potential in Colombia</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>This paper presents a novel method to estimate the future biomass energy potential in countries with domestic markets unable to influence international markets. As a study case, the biomass energy potential in Colombia is estimated for the period 2010–2030. The prediction model is a scenario-based optimization algorithm that maximizes the yearly profit of locally producing and importing commodities in a country subject to certain constraints (domestic demand, limited area, etc.) as well as to demographic, macroeconomic and market data (e.g. domestic and international prices of commodities). The bioenergy potential associated to the production of commodities is calculated according to a methodology presented by the same authors. In order to provide a modeling framework consistent with other state-of-the-art projections, global scenarios for analysis are selected from the literature rather than formulated. Selected global scenarios highlight the influence of global biofuel use on agricultural prices, production and demand. Results predict a theoretical bioenergy potential in Colombia 56%–69% larger in 2030 than in 2010 (1.31–1.41 EJ). A sensitivity analysis shows that while a higher global biofuel use leads to a higher local bioenergy potential, its influence is less pronounced than that of agricultural yields, demand and specific energy of biomass resources.</t>
+          <t>South Australian agriculture: a narrative to encourage future policy reform.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3164318489</t>
+          <t>https://openalex.org/W4283707183</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.emcon.2021.05.001</t>
+          <t>https://doi.org/10.1080/01440365.2022.2092944</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Oladele et al. (2021)</t>
+          <t>Hamilton (2022)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Emerging contaminants: Evaluation of degradable chelators towards enhancing cadmium phytoextraction efficiency of bioenergy crop grown on polluted soil</t>
+          <t>Equality Arguments, Contemporary Feminist Voices and the Matrimonial Causes Act 1923</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Exogenous application of chelators towards enhancing heavy metals extraction efficiency of bioenergy crop has received considerable attention in recent time. However, little is known about optimal application rate, comparative evaluation of degradable versus non-degradable chelators and their impact on cadmium (Cd) speciation and uptake, physiological and biochemical activity of sweet sorghum grown under Cd stress. Four chelators namely, Nitrilotriacetic acid (NTA), tetrasodium N,N-diacetate (TDA), Ethylenediamine tetraacetic acid (EDTA), iminodisuccinic acid (IDA) and control (CK) were applied and compared at rates of 2, 5, and 10 mmol kg−1 towards augmenting phytoextraction efficiency of sweet sorghum for Cd remediation in a screen house study. Results showed that sweet sorghum augmented with TDA significantly (P &lt; 0.05) increased biomass, enhanced Cd uptake and accumulation when compared to EDTA at application rate of 2–5 mmol kg−1. TDA influenced Cd speciation via increasing acid-soluble, reducible, oxidizable, and residual fractions of Cd, thus increasing Cd bioavailability. NTA and TDA increased proline concentrations, antioxidant enzymes and net photosynthetic activity rate (Pn) comparably to EDTA in sweet sorghum, thus enhancing stress tolerance and stabilizing photosynthetic activities. Overall, exogenous application of degradable TDA at 2–5 mmol kg−1 could be recommended as replacement for non-degradable EDTA in a chelate assisted approach towards augmenting bioenergy crop for phytoremediation of Cd polluted soil.</t>
+          <t>The Matrimonial Causes Act 1923 equalized the grounds for divorce for men and women, removing the prior existing double standard. Before this reform whilst husbands could divorce wives on the basis of adultery alone, wives had to prove additional aggravating factors. This author by analysis of primary sources from the National Union of Societies for Equal Citizenship archive, Hansard and the Royal Commission on Divorce and Matrimonial Causes Report 1912 demonstrates that some contemporaneous actors were persuaded by the symbolism of equality arguments and considered these convincing reasons for reform. This led to the enactment of the legislation in question. Yet in critical evaluation other feminists already recognized limitations with the reform achieved. Namely, that it distracted from other agendas, took too long, that poverty remained a barrier to reform and the reform achieved did not go far enough as the grounds for divorce were not reformed and there was no genuine commitment to equality for women within marriage. Others were prepared to adopt any strategy which led to reform seeing this as pragmatic first step.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3197358676</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.energy.2021.121953</t>
+          <t>https://openalex.org/W2349712766</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Wei et al. (2022)</t>
+          <t>Tie-yong (2004)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Modelling and experimental validation of an EV torque distribution strategy towards active safety and energy efficiency</t>
+          <t>Experiences &amp; Revelation of Citizen Moral Education in Developed Countries</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Electric vehicles (EVs) have promisingly contributed to the decarbonization of the transportation sector. Torque distribution in energy management is vital to enhance EV safety and efficiency; however, its nonlinearity and real-time executability have not been extensively researched. This paper proposes an integrated torque distribution strategy that simultaneously considers vehicle security and dynamic power allocation. In the upper active safety layer, the yaw stability control and active front steering control are coupled to maintain vehicle stability. Additionally, a linear time-varying model predictive controller is developed to address the system nonlinearity and online executability problems. In the lower energy distribution layer, the motor efficiency and dynamic tire-slip power are simultaneously optimized to maintain EV energy conservation. Numerical simulations and hardware experiments are conducted in this study. The results demonstrate that the proposed integrated strategy is superior to other typical torque distribution strategies in terms of reducing the risk of emergent accidents. Moreover, the energy consumption of the powertrain is reduced by 13.4% and 14.2% under the steering and straight driving conditions, respectively. Overall, our study further promotes the practical application of EVs in the future automotive market and lays a solid foundation for intelligent torque distribution in autonomous EVs.</t>
+          <t>From the experience accumulated by the developed countries about the moral education of the citizen in market economy and multiple cultures, we noticed the effective moral-education experience which takes the common value outlook as a core content, the association of scientific spirit with humanistic spirit as a basic principle, and makes full use of moral resources of national culture. It can play a significant part in China's moral-education reform and is worth further research and attention.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2924505825</t>
+          <t>https://openalex.org/W2079707064</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1787/906cea2b-en</t>
+          <t>https://doi.org/10.1186/1475-2875-7-98</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Gruère &amp; Boëdec (2019)</t>
+          <t>Khatib et al. (2008)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Navigating pathways to reform water policies in agriculture</t>
+          <t>Markets, voucher subsidies and free nets combine to achieve high bed net coverage in rural Tanzania</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>This report offers a guide on potential reform pathways towards sustainable agriculture water use, based on a thorough review of selected past water and agriculture reforms and extensive consultation with policy experts. A theory of change is developed that emphasises the importance of flexibility in the timing and design of reform processes to achieve practical and effective policy changes. Governments should prepare future reforms, via continued research, education, and governance efforts, to help take advantage of reform opportunities when the timing is right. Five necessary conditions are identified for a successful reform process: (i) support evidence-based problem definition, objective setting and evaluations; (ii) ensure that governance and institutions are aligned with the policy change; (iii) engage stakeholders strategically and build trust; (iv) rebalance economic incentives to mitigate short run economic losses; and (v) define an adjustable smart reform sequencing that provides flexibility in the long run. These conditions are found to be necessary to implement four challenging policy changes: charging water use in agriculture; removing subsidies that negatively impact water resources, regulating groundwater use and addressing nonpoint source pollution. But the relative effort that governments need to devote to fulfilling each of the five conditions will vary depending on the policy change.</t>
+          <t>Tanzania has a well-developed network of commercial ITN retailers. In 2004, the government introduced a voucher subsidy for pregnant women and, in mid 2005, helped distribute free nets to under-fives in small number of districts, including Rufiji on the southern coast, during a child health campaign. Contributions of these multiple insecticide-treated net delivery strategies existing at the same time and place to coverage in a poor rural community were assessed. Cross-sectional household survey in 6,331 members of randomly selected 1,752 households of 31 rural villages of Demographic Surveillance System in Rufiji district, Southern Tanzania was conducted in 2006. A questionnaire was administered to every consenting respondent about net use, treatment status and delivery mechanism. Net use was 62.7% overall, 87.2% amongst infants (0 to1 year), 81.8% amongst young children (&gt;1 to 5 years), 54.5% amongst older children (6 to 15 years) and 59.6% amongst adults (&gt;15 years). 30.2% of all nets had been treated six months prior to interview. The biggest source of nets used by infants was purchase from the private sector with a voucher subsidy (41.8%). Half of nets used by young children (50.0%) and over a third of those used by older children (37.2%) were obtained free of charge through the vaccination campaign. The largest source of nets amongst the population overall was commercial purchase (45.1% use) and was the primary means for protecting adults (60.2% use). All delivery mechanisms, especially sale of nets at full market price, under-served the poorest but no difference in equity was observed between voucher-subsidized and freely distributed nets. All three delivery strategies enabled a poor rural community to achieve net coverage high enough to yield both personal and community level protection for the entire population. Each of them reached their relevant target group and free nets only temporarily suppressed the net market, illustrating that in this setting that these are complementary rather than mutually exclusive approaches.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2054677294</t>
+          <t>https://openalex.org/W3034708674</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1353/cwh.1982.0057</t>
+          <t>https://doi.org/10.1111/boer.12239</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Scarborough (1982)</t>
+          <t>Lee &amp; Muminov (2020)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>&lt;i&gt;Edmund Ruffin: A Biography&lt;/i&gt; (review)</t>
+          <t>R&amp;amp;D Information sharing in a mixed duopoly and incentive subsidy for research joint venture competition</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>84CIVIL WAR HISTORY Edmund Ruffin: A Biography. By Betty L. Mitchell. (Bloomington: Indiana University Press, 1981. Pp. ?, 306. $22.50.) One would not expect a prote'gé of Stephen Oates, the biographer of such figures as John Brown, Nat Turner, and Abraham Lincoln, to display much sympathy for a southern fire-eater. And that is decidedlythe case with Betty Mitchell's new biography of Edmund Ruffin. At great pains to deny that her study is an"apologia or justification" ofRuffin lest she be tarnished by the unfashionable views of her central figure, the author announces at the outset that she will eschew psychoanalysis of this "essentially tragic figure" and simply let her readers form their own conclusions about him. Yet, in the narrative that follows, Mitchell manifests an attitude toward Ruffin which can best be characterized as uniformly and unremittingly unsympathetic, sarcastic, condescending, and sneering. In view of her ill-concealed dishke for thenoted agricultural reformer and dedicated southern nationalist, it is surprising that Mitchell would undertake a new life of Ruffin, especially since a superb study of the fiery Virginian already exists. Unfortunately, the present work is less satisfactory than the previous biography of Ruffin, written fifty years ago by Avery Craven, and adds Uttle to our understanding of either Ruffin or the society of which he was a part. Mitchell employs no new methodology, provides little analysis, offers no direct challenge to the interpretations of Craven (whom she does not mentionin either preface or text), and utilizes no significant new primary sources. Like Craven, she rehes very heavily on Ruffin's 4100-page manuscript diary, basing eight of her last nine chapters almost exclusively on that source. It is not clear to what extent her work was facilitated by the printed version of that diary, the first volume of which appeared more than two years before she commenced her study, since virtually all citations are to the manuscript diary. Incredibly, she seems unaware (judging by her bibliography ) that the second volume of the edited diary was published in 1977. To her credit, Mitchell is an imaginative and, attunes, brilliantwriter; indeed, her study of Ruffin reads almost like a novel. And therein lies another problem. Not only does she employ the styleofthe novelist, but also many of the techniques—devices which may be proper in abook of fiction but which have no place in a scholarly work. Thus, she extrapolates material from separate conversations and letters and passes them off as one in the text (pp. 99, 216-17); she attributes to Ruffin statements apparently made at one point in time which actually were written at other times (pp. 234, 248); she misrepresents evidence for narrative effect (p. 172, withrespectto theallegedinterruption ofRuffin's journey to Montgomery). More than this, the book is marred by imprecise wording, careless citation of sources (there are more than fifty such errors in references to the diary alone), and factual errors—it was William Boulware, not Baulwane (p. 79); Johnson J. Hooper, not Johnson A. (p. 159); Colonel Terry, not Ferry (p. 190); John Shdell, not BOOK REVIEWS85 Sliddell (p. 201); John Quincy Adams, not John Adams, was a presidential candidate in 1824 (p. 23); Ruffin was not in Washington on New Year's Eve, 1859 (p. 151); seceding southern delegatesnominated Breckinridge in Baltimore, not Richmond (p. 157); and the Confederate Congress did not pass a new conscription law in the summer of 1863 (p. 236). More serious is the consistent misreading of evidence to make Ruffin appear ludicrous, inept, self-serving, vain, and senile. Armed with a plethora of deprecatory words—he "clucked," he "whined," he "frothed," he was subject to "burping spells," he was a "martinet," he looked like "some queer apparition of the Ancient Mariner"—Mitchell labors assiduously to ridicule her subject. The same end is achieved through subtle manipulation of source materials. Thus, Ruffin's statement , "I spoke . . . for about three-quarters of an hour—&amp; then stopped, having forgotten to bring in some of my main points," becomes, in the hands of Mitchell: ". . . he rambled on for threequarters of an hour, then ended abruptly, having forgotten to mention most of his main points" (p. 167, my itaUcs). Considered individually, such examples...</t>
+          <t>Abstract This study investigates the incentives for R&amp;amp;D (research and development) information sharing in a mixed duopoly and finds a contrasting result that public firm chooses full sharing while private firm enjoys free‐riding. We then devise an agreement‐based incentive R&amp;amp;D subsidy scheme for RJV (research joint venture) competition, which can internalize R&amp;amp;D spillovers between firms and induce them to earn higher payoffs through full sharing of their R&amp;amp;D information. We also discuss welfare loss of the proposed R&amp;amp;D subsidy scheme, compare with production subsidy and provide some policy‐relevant implications on privatization.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4320496096</t>
+          <t>https://openalex.org/W4390908422</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://doi.org/10.3390/en16041833</t>
+          <t>https://doi.org/10.1186/s12937-023-00895-0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Karoń &amp; Tománek (2023)</t>
+          <t>Lee et al. (2024)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Effectiveness of Urban Mobility Decarbonization Instruments</t>
+          <t>Improving economic access to healthy diets in first nations communities in high-income, colonised countries: a systematic scoping review</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Decarbonization of urban mobility requires complex, interconnected actions. The instruments for decarbonizing urban mobility include urban collective transport, bicycles and means of personal transport, cybermobility and electromobility. The article presents the results of research on the transport behavior of the creative class, the effects of the COVID-19 pandemic on the functioning of urban mobility, and the results of research on the efficiency of electromobility in the field of the implementation of battery-powered buses. The research was aimed at a critical assessment of the current mobility model and creation of the basis for change in this area. In particular, these studies focused on changes in transport needs and greater use of cyberspace for various activities, which should reduce the volume of physical flows of people in urban transport networks. The aim of the article is to present the conclusions of these studies in terms of their use to change mobility models in cities. The practical significance of the presented research consists in indicating the factors of building individualized urban mobility strategies, with particular emphasis on the issues of sustainable development and decarbonization. The authors’ contribution to the development of science is demonstration of the possibilities of changing the mobility model in the city and reducing greenhouse gas emissions. In particular, this applies to urban metropolises that are moving away from heavy mining and processing industries, i.e., the number of jobs in business and educational services is increasing, and the industry of new technologies is developing. The conclusions formulated in the paper indicate, in particular, the significant decarbonization potential of cybermobility and the use of zero-emission means of transport, such as bicycles and scooters, which can be released by changing the approach to the organization of work and learning, in particular their virtualization and deconcentration of travel sources.</t>
+          <t>Abstract Background Affordability of healthy food is a key determinant of the diet-related health of First Nations Peoples. This systematic scoping review was commissioned by the Ngaanyatjarra Pitjantjatjara Yankunytjatjara Women’s Council (NPYWC) in Central Australia to identify interventions to improve economic access to healthy food in First Nations communities in selected high-income, colonised countries. Methods Eight databases and 22 websites were searched to identify studies of interventions and policies to improve economic access to healthy food in First Nations communities in Australia, Canada, the United States or New Zealand from 1996 to May 2022. Data from full text of articles meeting inclusion criteria were extracted to a spreadsheet. Results were collated by descriptive synthesis. Findings were examined with members of the NPYWC A n angu research team at a co-design workshop. Results Thirty-five publications met criteria for inclusion, mostly set in Australia (37%) or the US (31%). Interventions ( n = 21) were broadly categorised as price discounts on healthy food sold in communities ( n = 7); direct subsidies to retail stores, suppliers and producers ( n = 2); free healthy food and/or food vouchers provided to community members ( n = 7); increased financial support to community members ( n = 1); and other government strategies ( n = 4). Promising initiatives were: providing a box of food and vouchers for fresh produce; prescriptions for fresh produce; provision/promotion of subsidised healthy meals and snacks in community stores; direct funds transfer for food for children; offering discounted healthy foods from a mobile van; and programs increasing access to traditional foods. Providing subsidies directly to retail stores, suppliers and producers was least effective. Identified enablers of effective programs included community co-design and empowerment; optimal promotion of the program; and targeting a wide range of healthy foods, particularly traditional foods where possible. Common barriers in the least successful programs included inadequate study duration; inadequate subsidies; lack of supporting resources and infrastructure for cooking, food preparation and storage; and imposition of the program on communities. Conclusions The review identified 21 initiatives aimed at increasing affordability of healthy foods in First Nations communities, of which six were deemed promising. Five reflected the voices and experiences of members of the NPYWC A n angu research team and will be considered by communities for trial in Central Australia. Findings also highlight potential approaches to improve economic access to healthy foods in First Nations communities in other high-income colonised countries. Trial registration PROSPERO CRD42022328326.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3135725234</t>
+          <t>https://openalex.org/W2233214058</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://doi.org/10.5194/egusphere-egu21-9480</t>
+          <t>https://doi.org/10.22004/ag.econ.252825</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Carvalho et al. (2021)</t>
+          <t>Nakabayashi (2008)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>A review of the potential of nature-based solutions (NBS) to address the challenges of the water-energy-food nexus (WEF Nexus) in the coming decades</t>
+          <t>Property and Risk: Revisit to Peasant Economy in Modern Japan</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>&amp;amp;lt;p&amp;amp;gt;The water, energy, and food security nexus (WEF Nexus) is the interlinkage between water security, energy security, and food security. An increasing world population is projected to increase energy and food requirements, which will increase the need for freshwater drastically in the coming decades. Projected climate change impacts will aggravate water availability, especially in urban areas. Nature-based solutions (NBS) have proven to generate multiple benefits that defuse the expected merging tensions within the WEF Nexus. This paper outlines the theories, provides examples, and discusses the potential of NBS to address the future WEF Nexus. For this purpose we reviewed recent papers on the theories of WE, WF, EF, and WEF Nexus, we described and summarized 19 representative real-life case studies, and we identified the knowledge gap within the theory and the case studies. We provide quantitative potentials and qualitative benefits for NBS described in the literature over the past decades. Our review demonstrated the impressive potential of NBS to address the projected challenges within the WEF Nexus. The study concludes by recommending NBS for specific WEF Nexus challenges and highlighting the need for decision-makers to consider the implementation of NBS in urban planings.&amp;amp;lt;/p&amp;amp;gt;</t>
+          <t>In Japan, under the Tokugawa shogunate, 1603–1868, registered peasants were guaranteed their property right of their farmland, but regulations on farmland trades restricted their access to financial markets and they were allowed to pay land tax in kind, which meant peasants were shielded against risk from volatility of financial market, land market and commodity market. Under the regulatory shield, millions of peasant family continued to be owner farmers and wealth inequality was kept small. However, during the Meiji Restoration from 1868, the government redefined peasants’ claim as the full-fledged modern property right, fully deregulated the land and financial market, and obliged landowners to pay land tax by money. With owner-peasants directly exposed to market risks, the ratio of tenanted land increased from 30 percent in the 1870s to the 50 percent in the 1900s. Behind the drastic redistribution of landownership, there was a new role of landlords replacing regulations: shielding tenant farmers against market risk. This institutional feature of tenancy contract was originally discussed by a Marxian economist Moritaro Yamada in the 1930s, when the mechanism had begun to collapse in the Great Depression. We attempt to formulate risk sharing mechanism managed by landlords, motivated by Yamada’s work.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2062700177</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.ecolecon.2005.10.020</t>
+          <t>https://openalex.org/W610515060</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Глазырина et al. (2006)</t>
+          <t>Beargie (1992)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>The polluter pays principle and potential conflicts in society</t>
+          <t>EFFORT TO END SHIPBUILDING SUBSIDIES FAILS.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>The conventional implementation of polluter pays principle (PPP) in many countries is based on the use of an environmental tax, which is determined proportionally to the amount of emissions of the polluting substances. In this paper we show that this practice is not adequate because of its real negative impact if the pollutant accumulates to a stock in the environment. Using a specific mathematical model we find, that in many cases there is a danger of an unavoidable conflict between the interests of society as a whole and the interests of private business, generated by these procedures of PPP implementation. This paper also presents a mathematical formula which expresses the time period, when the conflict arises. We call it “the time boundary of investment expediency”. Some results of a numerical simulation for the calculation of this quantity for different investment initiatives are also presented in this article. On the basis of the model analysis, we suggest “a corrected” amount of environmental tax which covers the negative effect on social welfare. We find that it should be dependent on the lifetime of the production project, not only on the amount of emitted pollution. The study gives some practical tools for strengthening governance in the environmental sector and for the evaluation of investment initiatives from a “quality of growth” point of view.</t>
+          <t>8 ASUBTITLE: PARIS TALKS COLLAPSE WHEN EUROPE, JAPAN AND KOREA REFUSE TO GO ALONG WITH U.S. PROPOSALS.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4378901651</t>
+          <t>https://openalex.org/W4240037995</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1051/e3sconf/202338904003</t>
+          <t>https://doi.org/10.1353/tcc.2001.0001</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Onufrienko (2023)</t>
+          <t>Yao (2001)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Green bonds’ social license: Singapore case</t>
+          <t>Rediscovering Tao Xingzhi as an Educational and Social Revolutionary</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Green bonds are a viable tool for upturning the established energy producing principles from upside down, based upon the efforts applied from bottom-up rather than the traditional regulatory approach. The intention of this paper is to evaluate the validity and the efficiency of this mechanism in order to compose a scenario of its most probable future sophistication. The outcome seems to be quite promising, regardless of some downfalls on the way, however, the specifications of inflexible fossil fuel-based economies may not allow this mechanism into play that easily. One of the possible solutions in that case could be suggested by the progressive Singaporean framework, supporting green bonds’ advances comprehensively by incentivizing their presence in a hybrid manner both on legislative level and socially. The efficacy of such approach could be proven by time only in the long run, yet the current developments suggest for it to be one of the best practices worthy of reception not only by the energy recipients, but also by the energy producers with customized modifications along the way.</t>
+          <t>Rediscovering Tao Xingzhi as an Educational and Social Revolutionary by Yusheng Yao In the past twenty years Tao Xingzhi (1891-1946) has been without doubt the most studied and propagated modem educator in China, and his ideas on education are being widely applied in various reform projects throughout the country. I Although recent bursts of interest in Tao have resulted in a more detailed and nuanced picture of the educator and his work, the real Tao Xingzhi remains elusive. This has much to do with the eclectic nature of his theories and practices, which were broad in scope, unsystematic and ever-changing. In fact, Tao himself had difficulties in explaining the exact meaning and full implications of his theory of life education in simple and easily understandable terms.2 Tao borrowed freely from such disparate and even contradictory intellectual sources as Confucianism, Christianity, the philosophy of John Dewey, anarchism, Sun Zhongshan's "Three People's Principles" and Marxism. Many of his contemporary educators and colleagues of disparate ideologies also inspired him with new ideas and methods.3 But the fundamental source of Tao's thought was his own life experience and various education experiments. The complex interactions of these sources, influences and his own reforms pose a challenge for those attempting to categorize him. The analysts of Tao's theory and practice tend to fall into two camps: those who emphasize and those who minimize the· impact of John Dewey on him. Neither of these two perspectives provides a balanced view and a sufficiently comprehensive approach to reveal the full complexity of Tao's intellectual development, including his relationship with Dewey. In addition, few studies have recognized the importance of anarchist influence on Tao's theory of life education.4 Understanding of Tao is further complicated by his involvement with the politics of the Chinese Communist Party during his life and after his death. Thus the realities of Tao's theories and practices are more complex than most interpretations suggest, making yet another search for the real Tao as necessary as it is challenging. Tao's theory and practice of life education represented 'a radical discourse in the Chinese debate on modem education and national reconstruction. Characterized by populism, pragmatism and voluntarism, Tao's educational and social radicalism was in constant tension with Chinese modem education, Chinese Twentieth-Century China, Vol. 27, No.2 (April, 2002): 79-120 80 Twentieth-Century China intellectuals, and the Nationalist government. As an educational radical, Tao was critical both of elitist and impractical traditional education and what he considered its "foreignized" version dominant in China's new schools. His radical social vision of a class-less society, rooted in his understanding of Confucianism and Christianity, and cross-fertilized with Dewey's philosophy and Chinese revolutionary discourses of the twentieth century, enabled him to conceptualize a radical theory of life education in his Xiaozhuang experiment (19271930 ). Through life education, which would integrate mind and hands, education and life, school and society, Tao sought to create new men and women, a new society and a new world. Tao was a fascinating character for his unconventional life and career and his unique personality as well as for his daring ideas and experiments. Coming from a poor family, Tao received an excellent education with others' help and through his own efforts. He experienced dramatic identity crises and spiritual awakenings twice, and changed his name each time to advertise his new identities . He was also twice on the government's "wanted" list, in part because of his radicalism. A returned student from the United States, his colleagues regarded him "as the most Chinese of the returned students." Always at the forefront of China's new education, Tao was a pioneer in popular education and rural reconstruction as well as in formal education. His life and work can be understood as the search of a modem intellectual for a viable individual and national identity, and for proper means and strategies of national reconstruction. Tao's extraordinary life was further enhanced by his unusual legacy in the People's Republic of China (PRC). After his death from a hemorrhage in 1946, which was widely regarded as his ultimate sacrifice for the...</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://openalex.org/W298329754</t>
+          <t>https://openalex.org/W4390959157</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.5089/9781484382844.081</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Aakkula &amp; Kröger (2006)</t>
+          <t>NA (2019)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Implementation of policies for sustainable development in the context of CAP New challenges for research</t>
+          <t>World Economic Outlook, October 2018</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>This background note concentrates on the crucial role of implementation in a policy process. It offers a brief review to recent implementation research and identifies future research needs in the field of sustainable development and the implementation of the Common Agricultural Policy (CAP). The focus is on the policy measures of the second pillar of the CAP, because their role as the advocates of sustainable development is expected to grow in the future. Current policy implementation research and related discussion are focused on an ongoing change in policy-making and implementation. There is a shift from hierarchical and centrally steered government to more networked governance that supersedes traditional administrative borders and includes different actors from outside the public sector. There is clearly a need for enhanced multi-level governance, which aims to a closer connection and interaction between the EU, national, regional and local levels of administration. The adaptation of the ideas behind multi-level governance would advance the successful implementation of policies for sustainable development. The CAP can be seen as a measure which has a long tradition in the maintenance of economic sustainability of agriculture in Europe. However, the evolution of the CAP since the MacSharry reform in 1992 has gradually augmented the contribution of the CAP to the ecological and social dimensions of sustainability. The first pillar of the CAP is currently under both modulation and decoupling. Modulation, i.e. reduction of direct payments, has brought a transfer of funds from the first pillar to the second pillar. At the same time decoupling has removed the link between direct payments and production, causing changes in farmers’ incentives and economic production environment. The new core of the first pillar is decoupled single farm payment (SFP), which is conditional on cross-compliance with certain environmental, public health and animal welfare standards. Therefore, it can be argued that in the future the first pillar will contribute less to economic sustainability (due to modulation) and more to ecological sustainability (due to cross-compliance). As a result of modulation the economic significance of the second pillar will increase. The introduction of cross-compliance in connection with the SFP may, in turn, reduce the demand for environmental goods and services provided by the second pillar measures of which the most important are compensatory allowances for less favoured areas (LFA) and agri-environmental measures. Therefore, it can be argued that in the future the second pillar will contribute more to economic sustainability (due to modulation) and less to ecological sustainability (due to cross-compliance). Regarding the social dimension of sustainability, the CAP is predominantly aimed to serve interests of farmers and not other rural people. If the key element of social sustainability is considered to be rural viability, the CAP guarantees a minimum income level for farmers, which to some extent directly contributes to rural viability. However, in the second pillar, the future tendency will be to broaden the view of rural development and subsequently allocate more funds to non-agricultural purposes. In this respect, one of the key instruments is the LEADER Community Initiative, which concentrates on the promotion local rural development through the activities of the local action groups. 1</t>
+          <t>AbstractGlobal growth for 2018–19 is projected to remain steady at its 2017 level, but its pace is less vigorous than projected in April and it has become less balanced. Downside risks to global growth have risen in the past six months and the potential for upside surprises has receded. Global growth is projected at 3.7 percent for 2018–19—0.2 percentage point lower for both years than forecast in April. The downward revision reflects surprises that suppressed activity in early 2018 in some major advanced economies, the negative effects of the trade measures implemented or approved between April and mid-September, as well as a weaker outlook for some key emerging market and developing economies arising from country-specific factors, tighter financial conditions, geopolitical tensions, and higher oil import bills. The balance of risks to the global growth forecast has shifted to the downside in a context of elevated policy uncertainty. Several of the downside risks highlighted in the April 2018 World Economic Outlook (WEO)—such as rising trade barriers and a reversal of capital flows to emerging market economies with weaker fundamentals and higher political risk—have become more pronounced or have partially materialized. Meanwhile, the potential for upside surprises has receded, given the tightening of financial conditions in some parts of the world, higher trade costs, slow implementation of reforms recommended in the past, and waning growth momentum.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4242805411</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.32604/ee.2021.014641</t>
+          <t>https://openalex.org/W3173957576</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Wang et al. (2021)</t>
+          <t>James (1904)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Optimal Trading Decision-Making of Power Supply Chain under Renewable Portfolio Standards</t>
+          <t>Robins, Elizabeth, [1904] [June] [18]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Under the background of implementing renewable portfolio standards and the ever-improving tradable green certificate scheme, the increasingly environmentally-friendly preference of power users is leading to changes in electricity demand, which, in turn, is driving changes in the decision-making behaviors of various actors in the power supply chain. Based on this, with the goal of pursuing maximum profit, consumer-power-demand functions have been introduced with some consideration of the factors of consumer preference to establish an optimal profit model for each trading subject in non-cooperative states of the power supply chain, under the constraints of meeting renewable energy portfolio standards. Here, the optimal strategy of each trading subject is presented by adopting the reverse induction method. Furthermore, examples are used to analyze factors such as the influence of environmental protection preferences, quota ratios, price substitutions, and market demand as well as the optimal profit of each trading subject in view of providing a reference for the decision-making in the power supply chain trading subjects.</t>
+          <t>The Reform Club; envelope included. Text begins: Enchanted to come in tomorrow; PAW 6/14/05 (transcription note)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3183610585</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.33051/2500-2325-2021-2-91-107</t>
+          <t>https://openalex.org/W3125279890</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Zoidov &amp; Медков (2021)</t>
+          <t>Gaffeo &amp; Molinari (2016)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Prospects for decarbonizing the world economy in the process of formation and evolutionary development of innovative and industrial belts of trade routes of the XXI century</t>
+          <t>Taxing financial transactions in fundamentally heterogeneous markets</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>The research is aimed at identifying the prospects for decarbonizing the world economy in the process of formation and evolutionary development of innovative and industrial belts of trade routes of the XXI century. Goal. Analyze, develop and propose the main directions for the development of economic (innovation-industrial) belts of trade routes of the XXI century in order to decarbonize the world economy. Tasks. To identify the directions of decarbonization of the transportation process by rail. To determine the prospects for the use of automatic (unmanned) mobile equipment when moving along international transport corridors and the possibility of reducing energy consumption in transport. Critically evaluate the effectiveness of expanding the use of hydrogen-cell and biofuel vehicles in the development of transport and transit systems. Develop recommendations for ensuring the sustainable development of cargo transportation along the Northern Sea Route (NSR). To show the organizational and institutional preconditions for the decarbonization of the world economy. Methodology. The research uses the methods of evolutionary and institutional theory, the theory of production and technological balance of the economy and technical and economic structures, world system analysis, expert and analytical assessments. Results. A system of arguments has been developed to prove that the high-tech transformation of global transport and logistics processes based on the principles of inter-state and corporate partnership (ICP), the development of the transit economy (TE) and the innovation and industrial belts of trade routes of the XXI century, which contribute to the wide spread of environmentally friendly industries, will make a decisive contribution to the de-carbonization of the world economy and ensuring sustainable economic development. It is determined that the decarbonization of the world economy in general and transport and transit systems in particular fits organically and forms an integral part of the Belt and Road Initiative of the People's Republic of China (BRI) put forward in 2013, and is closely correlated with such important components of the BRI as the Digital Silk Road and the Silk Road of Health. Conclusions. The development of the economic (innovation-industrial) belts of trade routes of the XXI century has a significant impact on the decarbonization of the world economy. The development of hydropower and long-distance transmission of generated electricity, as well as the construction and modernization of global, regional and transit energy transport systems will contribute to reducing carbon dioxide emissions. When creating and operating the Norman-Aryan trade route of the XXI century, it is necessary to set the task of supplying electricity to transport communications and rolling stock exclusively from renewable energy sources (RES), and for the countries of Central Asia – through the use of hydropower, solar and wind sources. The construction and operation of the "Green Silk Road" will become a reliable ecological and innovative basis for the development of the transit economy in Russia and the countries of Central Asia.</t>
+          <t>The recent global financial crisis has revived a well-honored debate on the desirability and feasibility of taxing financial activities to curb speculation and promote price stability. In this paper we apply agent-based computational techniques to explore this issue in a multi-market environment in which the processes driving the fundamental value of the securities traded in different jurisdictions are heterogeneous. A natural exemplification is to assume that security dealers have the opportunity of submitting orders by choosing among stock markets at different stages of development. We argue that the proper policy objective to be targeted is not volatility in itself, but that in excess of the discounted stream of subsequent dividends, that is price efficiency. In this case, a global coordination is incentive-compatible, given that it minimizes the distortion associated to speculative trading on the one hand, and it ensures that the loss of trading volume is lower if compared to the case of unilateral taxation on the other one. Notwithstanding a fundamental heterogeneity of the markets involved, the optimal tax rate turns out to be uniform.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2013710807</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.2982/0012-8317(1998)87[339:tusppp]2.0.co;2</t>
+          <t>https://openalex.org/W3040919976</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Bhatia &amp; Buckley (1998)</t>
+          <t>Alshira’h (2018)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>The Uluguru Slopes Planning Project: Promoting Community Involvement in Biodiversity Conservation</t>
+          <t>Determinants of sales tax compliance among Jordanian SMEs : the moderating effect of public governance</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>The Uluguru Mountain forests of Eastern Tanzania are of high importance both for the conservation of biodiversity, and as a water catchment area for major urban centres. Only about 270 km2 of forest is thought to remain, mostly inside forest reserves. The most biologically valuable sub-montane forest has been badly affected by habitat destruction and only a small area in the north-east Ulugurus remains.The main objective of the Uluguru Slopes Planning Project was to research the resource utilisation practices of villagers and their attitudes to forest conservation in the Ulugurus, through a socio-economic survey using participatory techniques. The findings demonstrated both that local communities are aware of the importance of forest conservation and that excellent examples of sustainable land management do exist. The results of the survey fed in to the planning of a follow-up project (funded by DANIDA), a key element of which will be the dissemination of this best practice more widely around the mountains.</t>
+          <t>Tax compliance leads to reducing the fiscal deficit and public debt, thereby it provides funding to satisfy the economic and social development. Despite the extensive government’s efforts, the compliance of sales tax (typically known as value added tax globally) among the Small and Medium-sized Enterprises (SMEs) in Jordan is relatively low, thus, it negatively impacts the government revenues. Previous studies regarding the determinants of sales tax compliance among SMEs are limited and somewhat inconsistent. Therefore, the present study aimed at extending Fischer’s model that is built on the integration of both economic and socio-psychological theories in the context of sales tax compliance as well as examining the moderating role of the public governance and patriotism as a new construct to have better understanding on the determinants of sales tax compliance. This study hypothesised eight factors affecting sales tax compliance, as well as eight hypotheses on the moderating effects of public governance on such relationships. Using the quantitative approach, this study employed a self-administered questionnaire survey of 660 owner-managers of SMEs listed in the Jordan Chamber of Industry of which 212 responses were usable for analysis purpose. The Partial Least Squares (PLS) results revealed positive influence of tax audit, tax penalty, tax moral, tax fairness and patriotism on sales tax compliance and a negative effect of tax complexity on sales tax compliance respectively. Meanwhile, peer influence and tax rate do not demonstrate any significant influence on sales tax compliance. The findings also ascertained the considerable moderating effect of the public governance on the associations between tax audit, tax penalty, and peer influence on sales tax compliance. Besides extending the body of knowledge by providing a comprehensive model to explain how several interrelated factors influence sales tax compliance, the results offer insights on the determinants of sales tax compliance among SMEs.</t>
         </is>
       </c>
     </row>

</xml_diff>